<commit_message>
Add emission factors for coal PPs. Cleanup Carma inventories. Lower case dataset names.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-biofuels.xlsx
+++ b/premise/data/additional_inventories/lci-biofuels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BE0844-0C52-DA42-9F3B-C27E03401450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BEA56E-2F9A-9E48-B819-985832EDA14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">GREET!$A$1:$J$2872</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Pereira et al. 2019'!$A$1:$J$220</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="0.01" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3733,9 +3733,6 @@
     <t>There is a net co-production of electricity (0.8 kWh per kg of ethanol produced), but cancelled by the additional electricity needed for CO2 capture. In this case, the carbon from fermentation CO2 is captured, by using additional electricity (180 kWh/t CO2) for compression. The captured CO2 is then stored. This configuration is not part of the GREET database. It displaces demand for liquid carbon dioxide used in the chemical industry. System expansion performed.</t>
   </si>
   <si>
-    <t>CO2 storage/at wood burning power plant 20 MW, truck 25km, post, pipeline 200km, storage 1000m</t>
-  </si>
-  <si>
     <t>CO2 storage. 97.5% of fermentation CO2 captured.</t>
   </si>
   <si>
@@ -4061,6 +4058,9 @@
   </si>
   <si>
     <t>US ton to metric ton</t>
+  </si>
+  <si>
+    <t>carbon dioxide storage at wood burning power plant 20 MW post, pipeline 200km, storage 1000m</t>
   </si>
 </sst>
 </file>
@@ -4767,7 +4767,7 @@
         <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
@@ -6240,7 +6240,7 @@
         <v>449</v>
       </c>
       <c r="F32" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G32" t="s">
         <v>481</v>
@@ -7237,13 +7237,13 @@
     </row>
     <row r="53" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="C53" t="s">
         <v>558</v>
       </c>
       <c r="D53" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -7283,13 +7283,13 @@
     </row>
     <row r="54" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="C54" t="s">
         <v>558</v>
       </c>
       <c r="D54" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -7534,13 +7534,13 @@
     </row>
     <row r="59" spans="2:17" ht="16" x14ac:dyDescent="0.2">
       <c r="B59" s="2" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="C59" t="s">
         <v>558</v>
       </c>
       <c r="D59" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -7580,13 +7580,13 @@
     </row>
     <row r="60" spans="2:17" ht="16" x14ac:dyDescent="0.2">
       <c r="B60" s="2" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="C60" t="s">
         <v>558</v>
       </c>
       <c r="D60" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -7626,13 +7626,13 @@
     </row>
     <row r="61" spans="2:17" ht="16" x14ac:dyDescent="0.2">
       <c r="B61" s="2" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C61" t="s">
         <v>558</v>
       </c>
       <c r="D61" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -7672,13 +7672,13 @@
     </row>
     <row r="62" spans="2:17" ht="16" x14ac:dyDescent="0.2">
       <c r="B62" s="2" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="C62" t="s">
         <v>558</v>
       </c>
       <c r="D62" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -7718,7 +7718,7 @@
     </row>
     <row r="64" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B64" s="9" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="65" spans="2:16" x14ac:dyDescent="0.2">
@@ -8913,13 +8913,13 @@
     </row>
     <row r="86" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="C86" t="s">
         <v>558</v>
       </c>
       <c r="D86" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="E86">
         <v>1</v>
@@ -8971,13 +8971,13 @@
     </row>
     <row r="87" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="C87" t="s">
         <v>558</v>
       </c>
       <c r="D87" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="E87">
         <v>1</v>
@@ -9261,13 +9261,13 @@
     </row>
     <row r="92" spans="2:16" ht="16" x14ac:dyDescent="0.2">
       <c r="B92" s="2" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="C92" t="s">
         <v>558</v>
       </c>
       <c r="D92" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="E92">
         <v>1</v>
@@ -9319,13 +9319,13 @@
     </row>
     <row r="93" spans="2:16" ht="16" x14ac:dyDescent="0.2">
       <c r="B93" s="2" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="C93" t="s">
         <v>558</v>
       </c>
       <c r="D93" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="E93">
         <v>1</v>
@@ -9377,13 +9377,13 @@
     </row>
     <row r="94" spans="2:16" ht="16" x14ac:dyDescent="0.2">
       <c r="B94" s="2" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C94" t="s">
         <v>558</v>
       </c>
       <c r="D94" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="E94">
         <v>1</v>
@@ -9435,13 +9435,13 @@
     </row>
     <row r="95" spans="2:16" ht="16" x14ac:dyDescent="0.2">
       <c r="B95" s="2" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="C95" t="s">
         <v>558</v>
       </c>
       <c r="D95" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="E95">
         <v>1</v>
@@ -9530,7 +9530,7 @@
         <v>449</v>
       </c>
       <c r="F99" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G99" t="s">
         <v>481</v>
@@ -13499,8 +13499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J2872"/>
   <sheetViews>
-    <sheetView topLeftCell="A1473" zoomScale="131" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="A1485" sqref="A1485:XFD1485"/>
+    <sheetView tabSelected="1" topLeftCell="B2579" zoomScale="131" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="B2596" sqref="B2596"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13588,7 +13588,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -14031,12 +14031,12 @@
         <v>36</v>
       </c>
       <c r="G32" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B33" s="6">
         <f>0.708</f>
@@ -14046,13 +14046,13 @@
         <v>121</v>
       </c>
       <c r="E33" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F33" t="s">
         <v>36</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -14452,7 +14452,7 @@
         <v>20</v>
       </c>
       <c r="G58" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H58" s="2"/>
     </row>
@@ -14851,7 +14851,7 @@
         <v>20</v>
       </c>
       <c r="G83" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H83" s="2"/>
     </row>
@@ -14873,7 +14873,7 @@
         <v>20</v>
       </c>
       <c r="G84" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H84" s="2"/>
     </row>
@@ -15296,7 +15296,7 @@
         <v>20</v>
       </c>
       <c r="G110" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H110" s="2"/>
     </row>
@@ -15309,7 +15309,7 @@
         <v>1</v>
       </c>
       <c r="B113" s="58" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
@@ -15365,7 +15365,7 @@
         <v>11</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
@@ -15410,7 +15410,7 @@
     </row>
     <row r="124" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B124" s="6">
         <v>1</v>
@@ -15704,9 +15704,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A137" s="2" t="s">
-        <v>1041</v>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>1150</v>
       </c>
       <c r="B137" s="6">
         <f>((B25*B125)-Parameters!$B$15)*0.975</f>
@@ -15722,10 +15722,10 @@
         <v>20</v>
       </c>
       <c r="G137" t="s">
-        <v>1050</v>
-      </c>
-      <c r="H137" s="2" t="s">
-        <v>1041</v>
+        <v>1049</v>
+      </c>
+      <c r="H137" t="s">
+        <v>1150</v>
       </c>
     </row>
     <row r="138" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -15746,7 +15746,7 @@
         <v>20</v>
       </c>
       <c r="G138" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H138" s="2"/>
     </row>
@@ -15759,7 +15759,7 @@
         <v>1</v>
       </c>
       <c r="B140" s="58" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
@@ -15860,7 +15860,7 @@
     </row>
     <row r="151" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B151" s="6">
         <v>1</v>
@@ -16151,9 +16151,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="164" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A164" s="2" t="s">
-        <v>1041</v>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>1150</v>
       </c>
       <c r="B164" s="6">
         <f>((B25*B152)-Parameters!$B$15)*0.975</f>
@@ -16169,10 +16169,10 @@
         <v>20</v>
       </c>
       <c r="G164" t="s">
-        <v>1050</v>
-      </c>
-      <c r="H164" s="2" t="s">
-        <v>1041</v>
+        <v>1049</v>
+      </c>
+      <c r="H164" t="s">
+        <v>1150</v>
       </c>
     </row>
     <row r="165" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -16193,7 +16193,7 @@
         <v>20</v>
       </c>
       <c r="G165" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H165" s="2"/>
     </row>
@@ -16206,7 +16206,7 @@
         <v>1</v>
       </c>
       <c r="B167" s="58" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
@@ -16307,7 +16307,7 @@
     </row>
     <row r="178" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B178" s="6">
         <v>1</v>
@@ -16598,9 +16598,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="191" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A191" s="2" t="s">
-        <v>1041</v>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>1150</v>
       </c>
       <c r="B191" s="6">
         <f>((B25*B179)-Parameters!$B$15)*0.975</f>
@@ -16616,10 +16616,10 @@
         <v>20</v>
       </c>
       <c r="G191" t="s">
-        <v>1050</v>
-      </c>
-      <c r="H191" s="2" t="s">
-        <v>1041</v>
+        <v>1049</v>
+      </c>
+      <c r="H191" t="s">
+        <v>1150</v>
       </c>
     </row>
     <row r="192" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -16640,7 +16640,7 @@
         <v>20</v>
       </c>
       <c r="G192" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H192" s="2"/>
     </row>
@@ -17694,7 +17694,7 @@
         <v>1</v>
       </c>
       <c r="B263" s="58" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="264" spans="1:10" x14ac:dyDescent="0.2">
@@ -17792,7 +17792,7 @@
     </row>
     <row r="273" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="B273" s="6">
         <v>1</v>
@@ -17815,7 +17815,7 @@
     </row>
     <row r="274" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A274" s="65" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B274" s="6">
         <v>1.00057</v>
@@ -18041,7 +18041,7 @@
         <v>1</v>
       </c>
       <c r="B286" s="58" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="287" spans="1:10" x14ac:dyDescent="0.2">
@@ -18139,7 +18139,7 @@
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B296" s="6">
         <v>1</v>
@@ -18162,7 +18162,7 @@
     </row>
     <row r="297" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A297" s="65" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B297" s="6">
         <v>1.00057</v>
@@ -18388,7 +18388,7 @@
         <v>1</v>
       </c>
       <c r="B309" s="58" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="310" spans="1:10" x14ac:dyDescent="0.2">
@@ -18486,7 +18486,7 @@
     </row>
     <row r="319" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="B319" s="6">
         <v>1</v>
@@ -18509,7 +18509,7 @@
     </row>
     <row r="320" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A320" s="65" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B320" s="6">
         <v>1.00057</v>
@@ -19198,7 +19198,7 @@
         <v>36</v>
       </c>
       <c r="G359" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="360" spans="1:8" x14ac:dyDescent="0.2">
@@ -19885,7 +19885,7 @@
     </row>
     <row r="394" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B394" s="6">
         <f>1.305</f>
@@ -19895,13 +19895,13 @@
         <v>121</v>
       </c>
       <c r="E394" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F394" t="s">
         <v>36</v>
       </c>
       <c r="G394" s="8" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="395" spans="1:7" x14ac:dyDescent="0.2">
@@ -20250,7 +20250,7 @@
         <v>20</v>
       </c>
       <c r="G417" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H417" s="2"/>
     </row>
@@ -20601,7 +20601,7 @@
         <v>20</v>
       </c>
       <c r="G440" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H440" s="2"/>
     </row>
@@ -20618,7 +20618,7 @@
         <v>1</v>
       </c>
       <c r="B443" s="58" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="444" spans="1:8" x14ac:dyDescent="0.2">
@@ -20719,7 +20719,7 @@
     </row>
     <row r="454" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A454" s="2" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="B454" s="6">
         <v>1</v>
@@ -20956,7 +20956,7 @@
         <v>20</v>
       </c>
       <c r="G464" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="H464" t="s">
         <v>30</v>
@@ -20964,7 +20964,7 @@
     </row>
     <row r="465" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
       <c r="B465" s="6">
         <f>(($B$364*$B$455)-Parameters!$B$15)*(0.975)</f>
@@ -20980,7 +20980,7 @@
         <v>20</v>
       </c>
       <c r="H465" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="466" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -21001,7 +21001,7 @@
         <v>20</v>
       </c>
       <c r="G466" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H466" s="2"/>
     </row>
@@ -21424,7 +21424,7 @@
         <v>20</v>
       </c>
       <c r="G492" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H492" s="2"/>
     </row>
@@ -22940,7 +22940,7 @@
         <v>36</v>
       </c>
       <c r="G590" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="591" spans="1:8" x14ac:dyDescent="0.2">
@@ -23625,7 +23625,7 @@
     </row>
     <row r="625" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A625" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B625" s="6">
         <f>1.305</f>
@@ -23635,13 +23635,13 @@
         <v>121</v>
       </c>
       <c r="E625" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F625" t="s">
         <v>36</v>
       </c>
       <c r="G625" s="8" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="627" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -23987,7 +23987,7 @@
         <v>20</v>
       </c>
       <c r="G648" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H648" s="2"/>
     </row>
@@ -24338,7 +24338,7 @@
         <v>20</v>
       </c>
       <c r="G671" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H671" s="2"/>
     </row>
@@ -24713,7 +24713,7 @@
         <v>20</v>
       </c>
       <c r="G695" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H695" s="2"/>
     </row>
@@ -25945,7 +25945,7 @@
         <v>36</v>
       </c>
       <c r="G779" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="780" spans="1:8" x14ac:dyDescent="0.2">
@@ -26010,7 +26010,7 @@
     </row>
     <row r="783" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A783" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B783" s="6">
         <f>1.299</f>
@@ -26020,13 +26020,13 @@
         <v>121</v>
       </c>
       <c r="E783" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F783" t="s">
         <v>36</v>
       </c>
       <c r="G783" s="8" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="785" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -26376,7 +26376,7 @@
         <v>20</v>
       </c>
       <c r="G806" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H806" s="2"/>
     </row>
@@ -26729,7 +26729,7 @@
         <v>20</v>
       </c>
       <c r="G829" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H829" s="2"/>
     </row>
@@ -26742,7 +26742,7 @@
         <v>1</v>
       </c>
       <c r="B831" s="58" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="832" spans="1:8" x14ac:dyDescent="0.2">
@@ -26798,7 +26798,7 @@
         <v>11</v>
       </c>
       <c r="B838" s="6" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="839" spans="1:8" x14ac:dyDescent="0.2">
@@ -26843,7 +26843,7 @@
     </row>
     <row r="842" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A842" s="2" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="B842" s="6">
         <v>1</v>
@@ -27090,7 +27090,7 @@
     </row>
     <row r="853" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A853" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
       <c r="B853" s="6">
         <f>(($B$780*$B$820)-Parameters!$B$15)*(0.975)</f>
@@ -27106,7 +27106,7 @@
         <v>20</v>
       </c>
       <c r="H853" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="854" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -27127,7 +27127,7 @@
         <v>20</v>
       </c>
       <c r="G854" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H854" s="2"/>
     </row>
@@ -27504,7 +27504,7 @@
         <v>20</v>
       </c>
       <c r="G878" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H878" s="2"/>
     </row>
@@ -29042,7 +29042,7 @@
         <v>36</v>
       </c>
       <c r="G977" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="978" spans="1:7" x14ac:dyDescent="0.2">
@@ -29687,7 +29687,7 @@
     </row>
     <row r="1010" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1010" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B1010" s="6">
         <f>0.708</f>
@@ -29697,13 +29697,13 @@
         <v>121</v>
       </c>
       <c r="E1010" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F1010" t="s">
         <v>36</v>
       </c>
       <c r="G1010" s="8" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="1012" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -30100,7 +30100,7 @@
         <v>20</v>
       </c>
       <c r="G1035" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H1035" s="2"/>
     </row>
@@ -30499,7 +30499,7 @@
         <v>20</v>
       </c>
       <c r="G1060" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H1060" s="2"/>
     </row>
@@ -30922,7 +30922,7 @@
         <v>20</v>
       </c>
       <c r="G1086" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H1086" s="2"/>
     </row>
@@ -30935,7 +30935,7 @@
         <v>1</v>
       </c>
       <c r="B1089" s="58" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="1090" spans="1:8" x14ac:dyDescent="0.2">
@@ -31036,7 +31036,7 @@
     </row>
     <row r="1100" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1100" s="2" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="B1100" s="6">
         <v>1</v>
@@ -31332,7 +31332,7 @@
     </row>
     <row r="1113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1113" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
       <c r="B1113" s="6">
         <f>((B982*B1101)-Parameters!$B$15)*0.975</f>
@@ -31348,7 +31348,7 @@
         <v>20</v>
       </c>
       <c r="H1113" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="1114" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -31369,7 +31369,7 @@
         <v>20</v>
       </c>
       <c r="G1114" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H1114" s="2"/>
     </row>
@@ -31382,7 +31382,7 @@
         <v>1</v>
       </c>
       <c r="B1116" s="58" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="1117" spans="1:8" x14ac:dyDescent="0.2">
@@ -31483,7 +31483,7 @@
     </row>
     <row r="1127" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1127" s="2" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="B1127" s="6">
         <v>1</v>
@@ -31776,7 +31776,7 @@
     </row>
     <row r="1140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1140" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
       <c r="B1140" s="6">
         <f>((B982*B1128)-Parameters!$B$15)*0.975</f>
@@ -31792,7 +31792,7 @@
         <v>20</v>
       </c>
       <c r="H1140" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="1141" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -31813,7 +31813,7 @@
         <v>20</v>
       </c>
       <c r="G1141" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H1141" s="2"/>
     </row>
@@ -31826,7 +31826,7 @@
         <v>1</v>
       </c>
       <c r="B1143" s="58" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="1144" spans="1:8" x14ac:dyDescent="0.2">
@@ -31927,7 +31927,7 @@
     </row>
     <row r="1154" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1154" s="2" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="B1154" s="6">
         <v>1</v>
@@ -32220,7 +32220,7 @@
     </row>
     <row r="1167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1167" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
       <c r="B1167" s="6">
         <f>((B982*B1155)-Parameters!$B$15)*0.975</f>
@@ -32236,7 +32236,7 @@
         <v>20</v>
       </c>
       <c r="H1167" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="1168" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -32257,7 +32257,7 @@
         <v>20</v>
       </c>
       <c r="G1168" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H1168" s="2"/>
     </row>
@@ -33311,7 +33311,7 @@
         <v>1</v>
       </c>
       <c r="B1239" s="58" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="1240" spans="1:10" x14ac:dyDescent="0.2">
@@ -33409,7 +33409,7 @@
     </row>
     <row r="1249" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1249" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="B1249" s="6">
         <v>1</v>
@@ -33432,7 +33432,7 @@
     </row>
     <row r="1250" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1250" s="2" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="B1250" s="6">
         <v>1.00057</v>
@@ -33658,7 +33658,7 @@
         <v>1</v>
       </c>
       <c r="B1262" s="58" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="1263" spans="1:10" x14ac:dyDescent="0.2">
@@ -33756,7 +33756,7 @@
     </row>
     <row r="1272" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1272" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B1272" s="6">
         <v>1</v>
@@ -33779,7 +33779,7 @@
     </row>
     <row r="1273" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1273" s="2" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="B1273" s="6">
         <v>1.00057</v>
@@ -34005,7 +34005,7 @@
         <v>1</v>
       </c>
       <c r="B1285" s="58" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="1286" spans="1:10" x14ac:dyDescent="0.2">
@@ -34103,7 +34103,7 @@
     </row>
     <row r="1295" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1295" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="B1295" s="6">
         <v>1</v>
@@ -34126,7 +34126,7 @@
     </row>
     <row r="1296" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1296" s="2" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="B1296" s="6">
         <v>1.00057</v>
@@ -34661,7 +34661,7 @@
     </row>
     <row r="1329" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1329" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B1329" s="6">
         <f>(0.1592+0.0136+0.0326)</f>
@@ -34671,13 +34671,13 @@
         <v>121</v>
       </c>
       <c r="E1329" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F1329" t="s">
         <v>36</v>
       </c>
       <c r="G1329" s="8" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="1331" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -35071,7 +35071,7 @@
         <v>20</v>
       </c>
       <c r="G1354" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H1354" s="2"/>
     </row>
@@ -35467,7 +35467,7 @@
         <v>20</v>
       </c>
       <c r="G1379" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H1379" s="2"/>
     </row>
@@ -35887,7 +35887,7 @@
         <v>20</v>
       </c>
       <c r="G1405" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H1405" s="2"/>
     </row>
@@ -37011,7 +37011,7 @@
     </row>
     <row r="1485" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1485" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B1485" s="5">
         <f>B1484*(1-B1486)</f>
@@ -37437,7 +37437,7 @@
         <v>36</v>
       </c>
       <c r="G1505" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="1506" spans="1:7" x14ac:dyDescent="0.2">
@@ -38023,7 +38023,7 @@
     </row>
     <row r="1535" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1535" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B1535" s="6">
         <f>(0.1173+0.0481+0.011)</f>
@@ -38033,13 +38033,13 @@
         <v>121</v>
       </c>
       <c r="E1535" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F1535" t="s">
         <v>36</v>
       </c>
       <c r="G1535" s="8" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="1537" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -38304,7 +38304,7 @@
         <v>20</v>
       </c>
       <c r="G1554" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="H1554" s="2"/>
     </row>
@@ -38574,7 +38574,7 @@
         <v>20</v>
       </c>
       <c r="G1573" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="H1573" s="2"/>
     </row>
@@ -38868,7 +38868,7 @@
         <v>20</v>
       </c>
       <c r="G1593" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="H1593" s="2"/>
     </row>
@@ -38877,7 +38877,7 @@
         <v>1</v>
       </c>
       <c r="B1595" s="58" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="1596" spans="1:8" x14ac:dyDescent="0.2">
@@ -38933,7 +38933,7 @@
         <v>11</v>
       </c>
       <c r="B1602" s="6" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="1603" spans="1:8" x14ac:dyDescent="0.2">
@@ -38978,7 +38978,7 @@
     </row>
     <row r="1606" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1606" s="2" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B1606" s="6">
         <v>1</v>
@@ -39134,7 +39134,7 @@
         <v>20</v>
       </c>
       <c r="G1612" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="H1612" t="s">
         <v>30</v>
@@ -39142,7 +39142,7 @@
     </row>
     <row r="1613" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1613" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
       <c r="B1613" s="6">
         <f>((B1513*B1607)-Parameters!$B$15)*0.975</f>
@@ -39158,7 +39158,7 @@
         <v>20</v>
       </c>
       <c r="H1613" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="1614" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -39179,7 +39179,7 @@
         <v>20</v>
       </c>
       <c r="G1614" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="H1614" s="2"/>
     </row>
@@ -39192,7 +39192,7 @@
         <v>1</v>
       </c>
       <c r="B1616" s="58" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="1617" spans="1:8" x14ac:dyDescent="0.2">
@@ -39293,7 +39293,7 @@
     </row>
     <row r="1627" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1627" s="2" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B1627" s="6">
         <v>1</v>
@@ -39449,7 +39449,7 @@
         <v>20</v>
       </c>
       <c r="G1633" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="H1633" t="s">
         <v>30</v>
@@ -39457,7 +39457,7 @@
     </row>
     <row r="1634" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1634" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
       <c r="B1634" s="6">
         <f>((B1513*B1628)-Parameters!$B$15)*0.975</f>
@@ -39473,7 +39473,7 @@
         <v>20</v>
       </c>
       <c r="H1634" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="1635" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -39494,7 +39494,7 @@
         <v>20</v>
       </c>
       <c r="G1635" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="H1635" s="2"/>
     </row>
@@ -39507,7 +39507,7 @@
         <v>1</v>
       </c>
       <c r="B1637" s="58" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="1638" spans="1:8" x14ac:dyDescent="0.2">
@@ -39563,7 +39563,7 @@
         <v>11</v>
       </c>
       <c r="B1644" s="6" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="1645" spans="1:8" x14ac:dyDescent="0.2">
@@ -39608,7 +39608,7 @@
     </row>
     <row r="1648" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1648" s="2" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B1648" s="6">
         <v>1</v>
@@ -39772,7 +39772,7 @@
     </row>
     <row r="1655" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1655" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
       <c r="B1655" s="6">
         <f>((B1513*B1649)-Parameters!$B$15)*0.975</f>
@@ -39788,7 +39788,7 @@
         <v>20</v>
       </c>
       <c r="H1655" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="1656" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -39809,7 +39809,7 @@
         <v>20</v>
       </c>
       <c r="G1656" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="H1656" s="2"/>
     </row>
@@ -40867,7 +40867,7 @@
         <v>1</v>
       </c>
       <c r="B1728" s="58" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="1729" spans="1:10" x14ac:dyDescent="0.2">
@@ -40965,7 +40965,7 @@
     </row>
     <row r="1738" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1738" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B1738" s="6">
         <v>1</v>
@@ -40988,7 +40988,7 @@
     </row>
     <row r="1739" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1739" s="2" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B1739" s="6">
         <v>1.00057</v>
@@ -41214,7 +41214,7 @@
         <v>1</v>
       </c>
       <c r="B1751" s="58" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="1752" spans="1:10" x14ac:dyDescent="0.2">
@@ -41312,7 +41312,7 @@
     </row>
     <row r="1761" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1761" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="B1761" s="6">
         <v>1</v>
@@ -41335,7 +41335,7 @@
     </row>
     <row r="1762" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1762" s="2" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B1762" s="6">
         <v>1.00057</v>
@@ -41561,7 +41561,7 @@
         <v>1</v>
       </c>
       <c r="B1774" s="58" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="1775" spans="1:10" x14ac:dyDescent="0.2">
@@ -41659,7 +41659,7 @@
     </row>
     <row r="1784" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1784" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="B1784" s="6">
         <v>1</v>
@@ -41682,7 +41682,7 @@
     </row>
     <row r="1785" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1785" s="2" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B1785" s="6">
         <v>1.00057</v>
@@ -41978,7 +41978,7 @@
     </row>
     <row r="1806" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1806" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B1806" s="5">
         <f>B1805*(1-B1807)</f>
@@ -42427,7 +42427,7 @@
         <v>36</v>
       </c>
       <c r="G1827" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="1828" spans="1:7" x14ac:dyDescent="0.2">
@@ -42994,7 +42994,7 @@
     </row>
     <row r="1856" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1856" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B1856" s="6">
         <f>180*(B1805/1000)</f>
@@ -43004,13 +43004,13 @@
         <v>121</v>
       </c>
       <c r="E1856" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F1856" t="s">
         <v>36</v>
       </c>
       <c r="G1856" s="8" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="1858" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -45254,7 +45254,7 @@
     </row>
     <row r="2007" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2007" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B2007" s="5">
         <f>B2006*(1-B2008)</f>
@@ -45682,7 +45682,7 @@
         <v>36</v>
       </c>
       <c r="G2027" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="2028" spans="1:8" x14ac:dyDescent="0.2">
@@ -46249,7 +46249,7 @@
     </row>
     <row r="2056" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2056" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B2056" s="6">
         <f>180*(B2006/1000)</f>
@@ -46259,13 +46259,13 @@
         <v>121</v>
       </c>
       <c r="E2056" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F2056" t="s">
         <v>36</v>
       </c>
       <c r="G2056" s="8" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="2058" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -47805,7 +47805,7 @@
     </row>
     <row r="2168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2168" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B2168" s="5">
         <f>B2167*(1-B2169)</f>
@@ -48275,7 +48275,7 @@
         <v>36</v>
       </c>
       <c r="G2190" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="2191" spans="1:8" x14ac:dyDescent="0.2">
@@ -48842,7 +48842,7 @@
     </row>
     <row r="2219" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2219" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B2219" s="6">
         <f>180*(B2169/1000)</f>
@@ -48852,13 +48852,13 @@
         <v>121</v>
       </c>
       <c r="E2219" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F2219" t="s">
         <v>36</v>
       </c>
       <c r="G2219" s="8" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="2221" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -50868,7 +50868,7 @@
     </row>
     <row r="2360" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2360" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B2360" s="5">
         <f>B2359*(1-B2361)</f>
@@ -51408,7 +51408,7 @@
         <v>36</v>
       </c>
       <c r="G2385" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="2386" spans="1:7" x14ac:dyDescent="0.2">
@@ -52455,7 +52455,7 @@
     </row>
     <row r="2438" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2438" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B2438" s="6">
         <f>(0.7444+0.0637+0.1525)</f>
@@ -52465,13 +52465,13 @@
         <v>121</v>
       </c>
       <c r="E2438" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F2438" t="s">
         <v>36</v>
       </c>
       <c r="G2438" s="8" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="2440" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -52847,7 +52847,7 @@
         <v>20</v>
       </c>
       <c r="G2462" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="H2462" s="2"/>
     </row>
@@ -53228,7 +53228,7 @@
         <v>20</v>
       </c>
       <c r="G2486" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="H2486" s="2"/>
     </row>
@@ -53657,7 +53657,7 @@
         <v>20</v>
       </c>
       <c r="G2512" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="H2512" s="2"/>
     </row>
@@ -54041,7 +54041,7 @@
         <v>20</v>
       </c>
       <c r="G2536" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="H2536" s="2"/>
     </row>
@@ -54422,7 +54422,7 @@
         <v>20</v>
       </c>
       <c r="G2560" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="H2560" s="2"/>
     </row>
@@ -54875,7 +54875,7 @@
         <v>20</v>
       </c>
       <c r="G2587" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="H2587" s="2"/>
     </row>
@@ -55243,7 +55243,7 @@
     </row>
     <row r="2611" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2611" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
       <c r="B2611" s="6">
         <f>((B2381*B2601)-Parameters!$B$15)*0.975</f>
@@ -55259,10 +55259,10 @@
         <v>20</v>
       </c>
       <c r="G2611" t="s">
-        <v>1042</v>
+        <v>1150</v>
       </c>
       <c r="H2611" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="2612" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -55283,7 +55283,7 @@
         <v>20</v>
       </c>
       <c r="G2612" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="H2612" s="2"/>
     </row>
@@ -55648,7 +55648,7 @@
     </row>
     <row r="2636" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2636" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
       <c r="B2636" s="6">
         <f>((B2381*B2626)-Parameters!$B$15)*0.975</f>
@@ -55664,10 +55664,10 @@
         <v>20</v>
       </c>
       <c r="G2636" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="H2636" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="2637" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -55688,7 +55688,7 @@
         <v>20</v>
       </c>
       <c r="G2637" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="H2637" s="2"/>
     </row>
@@ -56125,7 +56125,7 @@
     </row>
     <row r="2664" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2664" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
       <c r="B2664" s="6">
         <f>((B2381*B2651)-Parameters!$B$15)*0.975</f>
@@ -56141,10 +56141,10 @@
         <v>20</v>
       </c>
       <c r="G2664" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="H2664" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="2665" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -56165,7 +56165,7 @@
         <v>20</v>
       </c>
       <c r="G2665" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="H2665" s="2"/>
     </row>
@@ -58260,7 +58260,7 @@
         <v>1</v>
       </c>
       <c r="B2805" s="58" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="2806" spans="1:10" x14ac:dyDescent="0.2">
@@ -58358,7 +58358,7 @@
     </row>
     <row r="2815" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2815" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="B2815" s="6">
         <v>1</v>
@@ -58607,7 +58607,7 @@
         <v>1</v>
       </c>
       <c r="B2828" s="58" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="2829" spans="1:10" x14ac:dyDescent="0.2">
@@ -58705,7 +58705,7 @@
     </row>
     <row r="2838" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2838" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="B2838" s="6">
         <v>1</v>
@@ -58954,7 +58954,7 @@
         <v>1</v>
       </c>
       <c r="B2851" s="58" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="2852" spans="1:10" x14ac:dyDescent="0.2">
@@ -59052,7 +59052,7 @@
     </row>
     <row r="2861" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2861" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B2861" s="6">
         <v>1</v>
@@ -59327,7 +59327,7 @@
   <dimension ref="A1:J220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -59412,7 +59412,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B10" s="5">
         <f>B9*(1-B11)</f>
@@ -60451,7 +60451,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B61" s="6">
         <f>(0.1173+0.0481+0.011)</f>
@@ -60461,13 +60461,13 @@
         <v>121</v>
       </c>
       <c r="E61" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F61" t="s">
         <v>36</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -60781,7 +60781,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B84" s="6">
         <f>(0.0867+0.0356+0.0081)</f>
@@ -60791,13 +60791,13 @@
         <v>121</v>
       </c>
       <c r="E84" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F84" t="s">
         <v>36</v>
       </c>
       <c r="G84" s="8" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -61134,7 +61134,7 @@
         <v>20</v>
       </c>
       <c r="G106" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H106" s="2"/>
     </row>
@@ -61472,7 +61472,7 @@
         <v>20</v>
       </c>
       <c r="G128" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H128" s="2"/>
     </row>
@@ -61834,7 +61834,7 @@
         <v>20</v>
       </c>
       <c r="G151" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H151" s="2"/>
     </row>
@@ -62896,8 +62896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J146"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="H121" sqref="H121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -62982,7 +62982,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B10" s="6">
         <f>B9*(1-B11)</f>
@@ -64101,7 +64101,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B65" s="6">
         <f>1.305</f>
@@ -64111,13 +64111,13 @@
         <v>121</v>
       </c>
       <c r="E65" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F65" t="s">
         <v>36</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -64519,7 +64519,7 @@
         <v>20</v>
       </c>
       <c r="G92" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H92" s="2"/>
     </row>
@@ -64528,7 +64528,7 @@
         <v>1</v>
       </c>
       <c r="B95" s="58" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
@@ -64629,7 +64629,7 @@
     </row>
     <row r="106" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="B106" s="6">
         <v>1</v>
@@ -64928,7 +64928,7 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
       <c r="B121" s="6">
         <f>4.2*0.975</f>
@@ -64944,7 +64944,7 @@
         <v>20</v>
       </c>
       <c r="H121" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -64965,7 +64965,7 @@
         <v>20</v>
       </c>
       <c r="G122" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H122" s="2"/>
     </row>
@@ -65335,8 +65335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N1112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A382" workbookViewId="0">
-      <selection activeCell="B421" sqref="B421"/>
+    <sheetView topLeftCell="A655" workbookViewId="0">
+      <selection activeCell="H697" sqref="H697"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -67684,7 +67684,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B120" s="6">
         <f>(1.1418+0.3058+0.1851)</f>
@@ -67694,13 +67694,13 @@
         <v>121</v>
       </c>
       <c r="E120" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F120" t="s">
         <v>36</v>
       </c>
       <c r="G120" s="8" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -68826,7 +68826,7 @@
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B190" s="6">
         <f>(0.0979+0.0262+0.0159)</f>
@@ -68836,13 +68836,13 @@
         <v>121</v>
       </c>
       <c r="E190" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F190" t="s">
         <v>36</v>
       </c>
       <c r="G190" s="8" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="192" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -69607,7 +69607,7 @@
         <v>20</v>
       </c>
       <c r="G222" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H222" s="2"/>
     </row>
@@ -71612,7 +71612,7 @@
     </row>
     <row r="330" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B330" s="6">
         <f>(0.7444+0.0637+0.1525)</f>
@@ -71622,13 +71622,13 @@
         <v>121</v>
       </c>
       <c r="E330" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F330" t="s">
         <v>36</v>
       </c>
       <c r="G330" s="8" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="332" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -72243,7 +72243,7 @@
         <v>20</v>
       </c>
       <c r="G362" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="H362" s="2"/>
     </row>
@@ -72668,7 +72668,7 @@
     </row>
     <row r="395" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B395" s="6">
         <f>B394*(1-B396)</f>
@@ -73073,7 +73073,7 @@
         <v>36</v>
       </c>
       <c r="G413" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="414" spans="1:8" x14ac:dyDescent="0.2">
@@ -73094,7 +73094,7 @@
         <v>36</v>
       </c>
       <c r="G414" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="415" spans="1:8" x14ac:dyDescent="0.2">
@@ -73115,7 +73115,7 @@
         <v>36</v>
       </c>
       <c r="G415" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="416" spans="1:8" x14ac:dyDescent="0.2">
@@ -73971,7 +73971,7 @@
     </row>
     <row r="458" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A458" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B458" s="6">
         <f>(0.0634+0.0201+0.0193)</f>
@@ -73981,13 +73981,13 @@
         <v>121</v>
       </c>
       <c r="E458" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F458" t="s">
         <v>36</v>
       </c>
       <c r="G458" s="8" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="460" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -74133,7 +74133,7 @@
         <v>20</v>
       </c>
       <c r="G471" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="H471" t="s">
         <v>647</v>
@@ -74372,7 +74372,7 @@
         <v>1</v>
       </c>
       <c r="B483" s="58" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="484" spans="1:8" x14ac:dyDescent="0.2">
@@ -74420,7 +74420,7 @@
         <v>11</v>
       </c>
       <c r="B489" s="6" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="490" spans="1:8" x14ac:dyDescent="0.2">
@@ -74473,7 +74473,7 @@
     </row>
     <row r="494" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A494" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B494" s="6">
         <v>1</v>
@@ -74781,7 +74781,7 @@
     </row>
     <row r="506" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A506" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
       <c r="B506" s="6">
         <f>(('Cozzolini 2018'!$B$471*'Cozzolini 2018'!$B$412)-Parameters!$B$15)*(0.975)</f>
@@ -74797,7 +74797,7 @@
         <v>20</v>
       </c>
       <c r="H506" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="508" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -75147,7 +75147,7 @@
         <v>1</v>
       </c>
       <c r="B530" s="58" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="531" spans="1:11" x14ac:dyDescent="0.2">
@@ -75240,7 +75240,7 @@
     </row>
     <row r="539" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A539" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="B539" s="6">
         <v>1</v>
@@ -75266,7 +75266,7 @@
     </row>
     <row r="540" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A540" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B540" s="6">
         <v>1.00057</v>
@@ -75739,7 +75739,7 @@
         <v>36</v>
       </c>
       <c r="G569" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="570" spans="1:8" x14ac:dyDescent="0.2">
@@ -75785,7 +75785,7 @@
     </row>
     <row r="572" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A572" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B572" s="6">
         <f>1.299</f>
@@ -75795,13 +75795,13 @@
         <v>121</v>
       </c>
       <c r="E572" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F572" t="s">
         <v>36</v>
       </c>
       <c r="G572" s="8" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="573" spans="1:8" x14ac:dyDescent="0.2">
@@ -76221,7 +76221,7 @@
         <v>20</v>
       </c>
       <c r="G596" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="H596" s="2"/>
     </row>
@@ -77422,7 +77422,7 @@
         <v>1</v>
       </c>
       <c r="B669" s="58" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="670" spans="1:8" x14ac:dyDescent="0.2">
@@ -77478,7 +77478,7 @@
         <v>11</v>
       </c>
       <c r="B676" s="6" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="677" spans="1:8" x14ac:dyDescent="0.2">
@@ -77523,7 +77523,7 @@
     </row>
     <row r="680" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A680" s="2" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="B680" s="6">
         <v>1</v>
@@ -77959,7 +77959,7 @@
     </row>
     <row r="697" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A697" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
       <c r="B697" s="6">
         <f>(Parameters!$B$16-(B652*B639))*(0.975)</f>
@@ -77975,7 +77975,7 @@
         <v>20</v>
       </c>
       <c r="H697" t="s">
-        <v>1041</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="699" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -79922,7 +79922,7 @@
     </row>
     <row r="803" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A803" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B803" s="6">
         <f>(1.1878+0.1611+0.2344)</f>
@@ -79932,13 +79932,13 @@
         <v>121</v>
       </c>
       <c r="E803" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="F803" t="s">
         <v>36</v>
       </c>
       <c r="G803" s="8" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="805" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -85561,7 +85561,7 @@
   <dimension ref="A2:H201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D221" sqref="D221"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -85574,7 +85574,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="58" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -85622,7 +85622,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -85630,18 +85630,18 @@
         <v>11</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B11" s="5"/>
     </row>
@@ -85655,7 +85655,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B13" s="28">
         <f>7059/(7059+554)</f>
@@ -85696,7 +85696,7 @@
     </row>
     <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
@@ -85866,7 +85866,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="B24" s="3">
         <f>(0.5+13.9)*$B$13*(Parameters!$B$5/7059)</f>
@@ -85882,7 +85882,7 @@
         <v>20</v>
       </c>
       <c r="H24" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -85929,7 +85929,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B27" s="3">
         <f>0.0000037*$B$13*(Parameters!$B$5/7059)</f>
@@ -85945,7 +85945,7 @@
         <v>20</v>
       </c>
       <c r="H27" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -86115,7 +86115,7 @@
         <v>1</v>
       </c>
       <c r="B38" s="58" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -86163,7 +86163,7 @@
         <v>9</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -86171,18 +86171,18 @@
         <v>11</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B46" s="5"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B47" s="5"/>
     </row>
@@ -86196,7 +86196,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B49" s="28">
         <f>7059/(7059+554)</f>
@@ -86237,7 +86237,7 @@
     </row>
     <row r="52" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="B52" s="3">
         <v>1</v>
@@ -86260,7 +86260,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B53" s="3">
         <f>1000*$B$49*(Parameters!$B$5/7059)</f>
@@ -86276,7 +86276,7 @@
         <v>20</v>
       </c>
       <c r="H53" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -86407,7 +86407,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="B60" s="3">
         <f>(0.5+13.9)*$B$49*(Parameters!$B$5/7059)</f>
@@ -86423,7 +86423,7 @@
         <v>20</v>
       </c>
       <c r="H60" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -86470,7 +86470,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B63" s="3">
         <f>0.0000037*$B$49*(Parameters!$B$5/7059)</f>
@@ -86486,7 +86486,7 @@
         <v>20</v>
       </c>
       <c r="H63" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -86656,7 +86656,7 @@
         <v>1</v>
       </c>
       <c r="B74" s="58" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -86680,7 +86680,7 @@
         <v>4</v>
       </c>
       <c r="B77" s="67" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -86704,7 +86704,7 @@
         <v>9</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -86715,13 +86715,13 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B82" s="5"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B83" s="5"/>
     </row>
@@ -86733,7 +86733,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B85" s="28">
         <f>5728/(5728+1514+2524)</f>
@@ -86774,7 +86774,7 @@
     </row>
     <row r="88" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B88" s="3">
         <v>1</v>
@@ -86792,7 +86792,7 @@
         <v>18</v>
       </c>
       <c r="H88" s="67" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -86902,7 +86902,7 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B94" s="3">
         <f>1.1*$B$85*(Parameters!B6/5728)</f>
@@ -86918,12 +86918,12 @@
         <v>20</v>
       </c>
       <c r="H94" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B95" s="3">
         <f>6.8*$B$85*(Parameters!B6/5728)</f>
@@ -86939,12 +86939,12 @@
         <v>20</v>
       </c>
       <c r="H95" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B96" s="3">
         <f>0.00000102*$B$85*(Parameters!B6/5728)</f>
@@ -86960,12 +86960,12 @@
         <v>20</v>
       </c>
       <c r="H96" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B97" s="3">
         <f>0.000000503*$B$85*(Parameters!B6/5728)</f>
@@ -86981,7 +86981,7 @@
         <v>20</v>
       </c>
       <c r="H97" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
@@ -87115,7 +87115,7 @@
         <v>1</v>
       </c>
       <c r="B106" s="58" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
@@ -87139,7 +87139,7 @@
         <v>4</v>
       </c>
       <c r="B109" s="67" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
@@ -87163,7 +87163,7 @@
         <v>9</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
@@ -87174,13 +87174,13 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B114" s="5"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B115" s="5"/>
     </row>
@@ -87192,7 +87192,7 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B117" s="28">
         <f>5728/(5728+1514+2524)</f>
@@ -87233,7 +87233,7 @@
     </row>
     <row r="120" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B120" s="3">
         <v>1</v>
@@ -87251,12 +87251,12 @@
         <v>18</v>
       </c>
       <c r="H120" s="67" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B121" s="3">
         <f>1000*$B$117*(Parameters!B6/5728)</f>
@@ -87272,7 +87272,7 @@
         <v>20</v>
       </c>
       <c r="H121" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
@@ -87361,7 +87361,7 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B126" s="3">
         <f>1.1*$B$117*(Parameters!B6/5728)</f>
@@ -87377,12 +87377,12 @@
         <v>20</v>
       </c>
       <c r="H126" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B127" s="3">
         <f>6.8*$B$117*(Parameters!B6/5728)</f>
@@ -87398,12 +87398,12 @@
         <v>20</v>
       </c>
       <c r="H127" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B128" s="3">
         <f>0.00000102*$B$117*(Parameters!B6/5728)</f>
@@ -87419,12 +87419,12 @@
         <v>20</v>
       </c>
       <c r="H128" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B129" s="3">
         <f>0.000000503*$B$117*(Parameters!B6/5728)</f>
@@ -87440,7 +87440,7 @@
         <v>20</v>
       </c>
       <c r="H129" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
@@ -87574,7 +87574,7 @@
         <v>1</v>
       </c>
       <c r="B139" s="58" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
@@ -87598,7 +87598,7 @@
         <v>4</v>
       </c>
       <c r="B142" s="67" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
@@ -87622,7 +87622,7 @@
         <v>9</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
@@ -87630,18 +87630,18 @@
         <v>11</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B147" s="5"/>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B148" s="5"/>
     </row>
@@ -87653,7 +87653,7 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="B150" s="28">
         <f>2524/(5728+1514+2524)</f>
@@ -87694,7 +87694,7 @@
     </row>
     <row r="153" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="B153" s="3">
         <v>1</v>
@@ -87712,7 +87712,7 @@
         <v>18</v>
       </c>
       <c r="H153" s="67" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
@@ -87822,7 +87822,7 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B159" s="3">
         <f>1.1*$B$150*(Parameters!B7/5728)</f>
@@ -87838,12 +87838,12 @@
         <v>20</v>
       </c>
       <c r="H159" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B160" s="3">
         <f>6.8*$B$150*(Parameters!B7/5728)</f>
@@ -87859,12 +87859,12 @@
         <v>20</v>
       </c>
       <c r="H160" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B161" s="3">
         <f>0.00000102*$B$150*(Parameters!B7/5728)</f>
@@ -87880,12 +87880,12 @@
         <v>20</v>
       </c>
       <c r="H161" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B162" s="3">
         <f>0.000000503*$B$150*(Parameters!B7/5728)</f>
@@ -87901,7 +87901,7 @@
         <v>20</v>
       </c>
       <c r="H162" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
@@ -88035,7 +88035,7 @@
         <v>1</v>
       </c>
       <c r="B171" s="58" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
@@ -88059,7 +88059,7 @@
         <v>4</v>
       </c>
       <c r="B174" s="67" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
@@ -88083,7 +88083,7 @@
         <v>9</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
@@ -88094,13 +88094,13 @@
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B179" s="5"/>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B180" s="5"/>
     </row>
@@ -88112,7 +88112,7 @@
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="B182" s="28">
         <f>2524/(5728+1514+2524)</f>
@@ -88153,7 +88153,7 @@
     </row>
     <row r="185" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="B185" s="3">
         <v>1</v>
@@ -88171,12 +88171,12 @@
         <v>18</v>
       </c>
       <c r="H185" s="67" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B186" s="3">
         <f>1000*$B$182*(Parameters!B7/5728)</f>
@@ -88192,7 +88192,7 @@
         <v>20</v>
       </c>
       <c r="H186" s="6" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
@@ -88281,7 +88281,7 @@
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B191" s="3">
         <f>1.1*$B$182*(Parameters!B7/5728)</f>
@@ -88297,12 +88297,12 @@
         <v>20</v>
       </c>
       <c r="H191" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B192" s="3">
         <f>6.8*$B$182*(Parameters!B7/5728)</f>
@@ -88318,12 +88318,12 @@
         <v>20</v>
       </c>
       <c r="H192" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B193" s="3">
         <f>0.00000102*$B$182*(Parameters!B7/5728)</f>
@@ -88339,12 +88339,12 @@
         <v>20</v>
       </c>
       <c r="H193" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B194" s="3">
         <f>0.000000503*$B$182*(Parameters!B7/5728)</f>
@@ -88360,7 +88360,7 @@
         <v>20</v>
       </c>
       <c r="H194" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.2">
@@ -88550,7 +88550,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B6">
         <v>37.200000000000003</v>
@@ -88558,7 +88558,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="B7">
         <v>43</v>
@@ -88640,7 +88640,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B17">
         <v>3.15</v>
@@ -88648,7 +88648,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="B18">
         <v>0.90700000000000003</v>

</xml_diff>

<commit_message>
Biofuels inventories were not importing correctly.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-biofuels.xlsx
+++ b/premise/data/additional_inventories/lci-biofuels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BEA56E-2F9A-9E48-B819-985832EDA14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75459A95-8298-C744-84C1-6C2259E03C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Parameters" sheetId="2" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Cavalett &amp; Cherubini 2022'!$A$2:$H$201</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Cavalett &amp; Cherubini 2022'!$A$1:$H$200</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Cozzolini 2018'!$A$1:$N$1112</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Gonzalez-Garcia et al. 2012'!$A$1:$J$146</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">GREET!$A$1:$J$2872</definedName>
@@ -7249,7 +7249,7 @@
         <v>1</v>
       </c>
       <c r="F53" s="35">
-        <f>'Cavalett &amp; Cherubini 2022'!B17</f>
+        <f>'Cavalett &amp; Cherubini 2022'!B16</f>
         <v>3.901221594640746</v>
       </c>
       <c r="G53" s="36">
@@ -7265,7 +7265,7 @@
         <v>0</v>
       </c>
       <c r="M53" s="5">
-        <f>'Cavalett &amp; Cherubini 2022'!B28</f>
+        <f>'Cavalett &amp; Cherubini 2022'!B27</f>
         <v>5.1810216734533041</v>
       </c>
       <c r="N53">
@@ -7295,7 +7295,7 @@
         <v>1</v>
       </c>
       <c r="F54" s="35">
-        <f>'Cavalett &amp; Cherubini 2022'!B53</f>
+        <f>'Cavalett &amp; Cherubini 2022'!B52</f>
         <v>3.901221594640746</v>
       </c>
       <c r="G54" s="36">
@@ -7311,7 +7311,7 @@
         <v>0</v>
       </c>
       <c r="M54" s="5">
-        <f>'Cavalett &amp; Cherubini 2022'!B64</f>
+        <f>'Cavalett &amp; Cherubini 2022'!B63</f>
         <v>5.1810216734533041</v>
       </c>
       <c r="N54">
@@ -7546,7 +7546,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="35">
-        <f>'Cavalett &amp; Cherubini 2022'!B89</f>
+        <f>'Cavalett &amp; Cherubini 2022'!B88</f>
         <v>3.8091337292647962</v>
       </c>
       <c r="G59" s="36">
@@ -7562,7 +7562,7 @@
         <v>0</v>
       </c>
       <c r="M59" s="5">
-        <f>'Cavalett &amp; Cherubini 2022'!B98</f>
+        <f>'Cavalett &amp; Cherubini 2022'!B97</f>
         <v>4.0775445422895764</v>
       </c>
       <c r="N59">
@@ -7592,7 +7592,7 @@
         <v>1</v>
       </c>
       <c r="F60" s="35">
-        <f>'Cavalett &amp; Cherubini 2022'!B121</f>
+        <f>'Cavalett &amp; Cherubini 2022'!B120</f>
         <v>3.8091337292647962</v>
       </c>
       <c r="G60" s="36">
@@ -7608,7 +7608,7 @@
         <v>0</v>
       </c>
       <c r="M60" s="5">
-        <f>'Cavalett &amp; Cherubini 2022'!B130</f>
+        <f>'Cavalett &amp; Cherubini 2022'!B129</f>
         <v>4.0775445422895764</v>
       </c>
       <c r="N60">
@@ -7638,7 +7638,7 @@
         <v>1</v>
       </c>
       <c r="F61" s="35">
-        <f>'Cavalett &amp; Cherubini 2022'!B154</f>
+        <f>'Cavalett &amp; Cherubini 2022'!B153</f>
         <v>1.9401623692733996</v>
       </c>
       <c r="G61" s="36">
@@ -7654,7 +7654,7 @@
         <v>0</v>
       </c>
       <c r="M61" s="5">
-        <f>'Cavalett &amp; Cherubini 2022'!B163</f>
+        <f>'Cavalett &amp; Cherubini 2022'!B162</f>
         <v>0.37850862891855597</v>
       </c>
       <c r="N61">
@@ -7684,7 +7684,7 @@
         <v>1</v>
       </c>
       <c r="F62" s="35">
-        <f>'Cavalett &amp; Cherubini 2022'!B186</f>
+        <f>'Cavalett &amp; Cherubini 2022'!B185</f>
         <v>1.9401623692733996</v>
       </c>
       <c r="G62" s="36">
@@ -7700,7 +7700,7 @@
         <v>0</v>
       </c>
       <c r="M62" s="5">
-        <f>'Cavalett &amp; Cherubini 2022'!B195</f>
+        <f>'Cavalett &amp; Cherubini 2022'!B194</f>
         <v>0.37850862891855597</v>
       </c>
       <c r="N62">
@@ -13194,7 +13194,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G101:G113">
-    <cfRule type="colorScale" priority="83">
+    <cfRule type="colorScale" priority="82">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -13202,7 +13202,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="82">
+    <cfRule type="colorScale" priority="83">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -13292,7 +13292,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:J28">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -13300,7 +13300,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -13499,7 +13499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J2872"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2579" zoomScale="131" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView topLeftCell="B2579" zoomScale="131" zoomScaleNormal="78" workbookViewId="0">
       <selection activeCell="B2596" sqref="B2596"/>
     </sheetView>
   </sheetViews>
@@ -85558,10 +85558,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F5820A-E001-4A42-8382-32FC181BB2BB}">
-  <dimension ref="A2:H201"/>
+  <dimension ref="A1:H200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -85569,137 +85569,161 @@
     <col min="1" max="1" width="75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B1" s="58" t="s">
         <v>1086</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="59" t="s">
-        <v>990</v>
+        <v>5</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>1110</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>1110</v>
+        <v>11</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1083</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>1083</v>
-      </c>
+        <v>1087</v>
+      </c>
+      <c r="B9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="B10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1088</v>
-      </c>
-      <c r="B11" s="5"/>
+        <v>485</v>
+      </c>
+      <c r="B11" s="66">
+        <v>0.31900000000000001</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>485</v>
-      </c>
-      <c r="B12" s="66">
-        <v>0.31900000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
         <v>1085</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B12" s="28">
         <f>7059/(7059+554)</f>
         <v>0.92722973860501778</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>14</v>
+        <v>1086</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>558</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="G15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="H15" s="59" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1086</v>
+        <v>69</v>
       </c>
       <c r="B16" s="3">
-        <v>1</v>
+        <f>1000*$B$12*(Parameters!$B$5/7059)</f>
+        <v>3.901221594640746</v>
       </c>
       <c r="C16" t="s">
         <v>558</v>
@@ -85708,64 +85732,61 @@
         <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="59" t="s">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>69</v>
+        <v>20</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="55" t="s">
+        <v>603</v>
       </c>
       <c r="B17" s="3">
-        <f>1000*$B$13*(Parameters!$B$5/7059)</f>
-        <v>3.901221594640746</v>
+        <f>6.9*$B$12*(Parameters!$B$5/7059)</f>
+        <v>2.691842900302115E-2</v>
       </c>
       <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="55" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>252</v>
+      </c>
+      <c r="B18" s="3">
+        <f>23.8*$B$12*(Parameters!$B$5/7059)</f>
+        <v>9.2849073952449762E-2</v>
+      </c>
+      <c r="C18" t="s">
         <v>558</v>
       </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="55" t="s">
-        <v>603</v>
-      </c>
-      <c r="B18" s="3">
-        <f>6.9*$B$13*(Parameters!$B$5/7059)</f>
-        <v>2.691842900302115E-2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>26</v>
-      </c>
       <c r="D18" t="s">
         <v>8</v>
       </c>
       <c r="F18" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="55" t="s">
-        <v>304</v>
+      <c r="H18" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B19" s="3">
-        <f>23.8*$B$13*(Parameters!$B$5/7059)</f>
-        <v>9.2849073952449762E-2</v>
+        <f>12.6*$B$12*(Parameters!$B$5/7059)</f>
+        <v>4.9155392092473403E-2</v>
       </c>
       <c r="C19" t="s">
         <v>558</v>
@@ -85777,19 +85798,19 @@
         <v>20</v>
       </c>
       <c r="H19" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>254</v>
+        <v>376</v>
       </c>
       <c r="B20" s="3">
-        <f>12.6*$B$13*(Parameters!$B$5/7059)</f>
-        <v>4.9155392092473403E-2</v>
+        <f>27*$B$12*(Parameters!$B$5/7059)</f>
+        <v>0.10533298305530014</v>
       </c>
       <c r="C20" t="s">
-        <v>558</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
         <v>8</v>
@@ -85798,19 +85819,19 @@
         <v>20</v>
       </c>
       <c r="H20" t="s">
-        <v>256</v>
+        <v>377</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>376</v>
+        <v>626</v>
       </c>
       <c r="B21" s="3">
-        <f>27*$B$13*(Parameters!$B$5/7059)</f>
-        <v>0.10533298305530014</v>
+        <f>10.7*$B$12*(Parameters!$B$5/7059)</f>
+        <v>4.1743071062655977E-2</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>558</v>
       </c>
       <c r="D21" t="s">
         <v>8</v>
@@ -85819,16 +85840,16 @@
         <v>20</v>
       </c>
       <c r="H21" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>626</v>
+        <v>628</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="55" t="s">
+        <v>601</v>
       </c>
       <c r="B22" s="3">
-        <f>10.7*$B$13*(Parameters!$B$5/7059)</f>
-        <v>4.1743071062655977E-2</v>
+        <f>1.7*$B$12*(Parameters!$B$5/7059)</f>
+        <v>6.6320767108892682E-3</v>
       </c>
       <c r="C22" t="s">
         <v>558</v>
@@ -85839,20 +85860,20 @@
       <c r="F22" t="s">
         <v>20</v>
       </c>
-      <c r="H22" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="55" t="s">
-        <v>601</v>
+      <c r="H22" s="56" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>1081</v>
       </c>
       <c r="B23" s="3">
-        <f>1.7*$B$13*(Parameters!$B$5/7059)</f>
-        <v>6.6320767108892682E-3</v>
+        <f>(0.5+13.9)*$B$12*(Parameters!$B$5/7059)</f>
+        <v>5.6177590962826741E-2</v>
       </c>
       <c r="C23" t="s">
-        <v>558</v>
+        <v>26</v>
       </c>
       <c r="D23" t="s">
         <v>8</v>
@@ -85860,20 +85881,20 @@
       <c r="F23" t="s">
         <v>20</v>
       </c>
-      <c r="H23" s="56" t="s">
-        <v>602</v>
+      <c r="H23" t="s">
+        <v>1082</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>1081</v>
+        <v>338</v>
       </c>
       <c r="B24" s="3">
-        <f>(0.5+13.9)*$B$13*(Parameters!$B$5/7059)</f>
-        <v>5.6177590962826741E-2</v>
+        <f>1766*$B$12*(Parameters!$B$5/7059)</f>
+        <v>6.8895573361355575</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>610</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
@@ -85882,40 +85903,40 @@
         <v>20</v>
       </c>
       <c r="H24" t="s">
-        <v>1082</v>
+        <v>339</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>338</v>
+        <v>294</v>
       </c>
       <c r="B25" s="3">
-        <f>1766*$B$13*(Parameters!$B$5/7059)</f>
-        <v>6.8895573361355575</v>
+        <f>0.00000000822*$B$12*(Parameters!$B$5/7059)</f>
+        <v>3.2068041507946933E-11</v>
       </c>
       <c r="C25" t="s">
-        <v>610</v>
+        <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="s">
         <v>20</v>
       </c>
       <c r="H25" t="s">
-        <v>339</v>
+        <v>295</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>294</v>
+        <v>1084</v>
       </c>
       <c r="B26" s="3">
-        <f>0.00000000822*$B$13*(Parameters!$B$5/7059)</f>
-        <v>3.2068041507946933E-11</v>
+        <f>0.0000037*$B$12*(Parameters!$B$5/7059)</f>
+        <v>1.4434519900170761E-8</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>558</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
@@ -85924,37 +85945,34 @@
         <v>20</v>
       </c>
       <c r="H26" t="s">
-        <v>295</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>1084</v>
+        <v>265</v>
       </c>
       <c r="B27" s="3">
-        <f>0.0000037*$B$13*(Parameters!$B$5/7059)</f>
-        <v>1.4434519900170761E-8</v>
-      </c>
-      <c r="C27" t="s">
-        <v>558</v>
+        <f>('Cavalett &amp; Cherubini 2022'!B16*'Cozzolini 2018'!$B$570)-Parameters!$B$15</f>
+        <v>5.1810216734533041</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
       </c>
       <c r="F27" t="s">
-        <v>20</v>
-      </c>
-      <c r="H27" t="s">
-        <v>1084</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>265</v>
-      </c>
-      <c r="B28" s="3">
-        <f>('Cavalett &amp; Cherubini 2022'!B17*'Cozzolini 2018'!$B$570)-Parameters!$B$15</f>
-        <v>5.1810216734533041</v>
+        <v>191</v>
+      </c>
+      <c r="B28" s="6">
+        <f>0.601*$B$12*(Parameters!$B$5/7059)</f>
+        <v>2.3446341783790884E-3</v>
       </c>
       <c r="D28" t="s">
         <v>8</v>
@@ -85968,11 +85986,11 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B29" s="6">
-        <f>0.601*$B$13*(Parameters!$B$5/7059)</f>
-        <v>2.3446341783790884E-3</v>
+        <f>0.3*$B$12*(Parameters!$B$5/7059)</f>
+        <v>1.1703664783922238E-3</v>
       </c>
       <c r="D29" t="s">
         <v>8</v>
@@ -85986,11 +86004,11 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>193</v>
+        <v>38</v>
       </c>
       <c r="B30" s="6">
-        <f>0.3*$B$13*(Parameters!$B$5/7059)</f>
-        <v>1.1703664783922238E-3</v>
+        <f>0.263*$B$12*(Parameters!$B$5/7059)</f>
+        <v>1.0260212793905162E-3</v>
       </c>
       <c r="D30" t="s">
         <v>8</v>
@@ -86004,11 +86022,11 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>314</v>
       </c>
       <c r="B31" s="6">
-        <f>0.263*$B$13*(Parameters!$B$5/7059)</f>
-        <v>1.0260212793905162E-3</v>
+        <f>0.00207*$B$12*(Parameters!$B$5/7059)</f>
+        <v>8.0755287009063426E-6</v>
       </c>
       <c r="D31" t="s">
         <v>8</v>
@@ -86022,11 +86040,11 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B32" s="6">
-        <f>0.00207*$B$13*(Parameters!$B$5/7059)</f>
-        <v>8.0755287009063426E-6</v>
+        <f>0.000563*$B$12*(Parameters!$B$5/7059)</f>
+        <v>2.19638775778274E-6</v>
       </c>
       <c r="D32" t="s">
         <v>8</v>
@@ -86040,11 +86058,11 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B33" s="6">
-        <f>0.000563*$B$13*(Parameters!$B$5/7059)</f>
-        <v>2.19638775778274E-6</v>
+        <f>0.0477*$B$12*(Parameters!$B$5/7059)</f>
+        <v>1.8608827006436358E-4</v>
       </c>
       <c r="D33" t="s">
         <v>8</v>
@@ -86058,11 +86076,11 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>312</v>
+        <v>40</v>
       </c>
       <c r="B34" s="6">
-        <f>0.0477*$B$13*(Parameters!$B$5/7059)</f>
-        <v>1.8608827006436358E-4</v>
+        <f>0.0271*$B$12*(Parameters!$B$5/7059)</f>
+        <v>1.0572310521476422E-4</v>
       </c>
       <c r="D34" t="s">
         <v>8</v>
@@ -86076,11 +86094,11 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>168</v>
       </c>
       <c r="B35" s="6">
-        <f>0.0271*$B$13*(Parameters!$B$5/7059)</f>
-        <v>1.0572310521476422E-4</v>
+        <f>0.0000903*$B$12*(Parameters!$B$5/7059)</f>
+        <v>3.5228030999605938E-7</v>
       </c>
       <c r="D35" t="s">
         <v>8</v>
@@ -86092,155 +86110,161 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>168</v>
-      </c>
-      <c r="B36" s="6">
-        <f>0.0000903*$B$13*(Parameters!$B$5/7059)</f>
-        <v>3.5228030999605938E-7</v>
-      </c>
-      <c r="D36" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" t="s">
-        <v>37</v>
-      </c>
-      <c r="F36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="58" t="s">
+      <c r="B37" s="58" t="s">
         <v>1089</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="B39" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>3</v>
-      </c>
-      <c r="B40" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="B40" s="59" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="59" t="s">
-        <v>990</v>
+        <v>5</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>7</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>1110</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>9</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>1110</v>
+        <v>11</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>1083</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>11</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>1083</v>
-      </c>
+        <v>1087</v>
+      </c>
+      <c r="B45" s="5"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="B46" s="5"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>1088</v>
-      </c>
-      <c r="B47" s="5"/>
+        <v>485</v>
+      </c>
+      <c r="B47" s="66">
+        <v>0.31900000000000001</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>485</v>
-      </c>
-      <c r="B48" s="66">
-        <v>0.31900000000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
         <v>1085</v>
       </c>
-      <c r="B49" s="28">
+      <c r="B48" s="28">
         <f>7059/(7059+554)</f>
         <v>0.92722973860501778</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+    <row r="49" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B50" s="6"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B49" s="6"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" t="s">
+        <v>5</v>
+      </c>
+      <c r="G50" t="s">
+        <v>11</v>
+      </c>
+      <c r="H50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>13</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>14</v>
+        <v>1089</v>
+      </c>
+      <c r="B51" s="3">
+        <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>2</v>
+        <v>558</v>
       </c>
       <c r="D51" t="s">
-        <v>7</v>
-      </c>
-      <c r="E51" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F51" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="G51" t="s">
-        <v>11</v>
-      </c>
-      <c r="H51" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="H51" s="59" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="B52" s="3">
-        <v>1</v>
+        <f>1000*$B$48*(Parameters!$B$5/7059)</f>
+        <v>3.901221594640746</v>
       </c>
       <c r="C52" t="s">
         <v>558</v>
@@ -86249,64 +86273,61 @@
         <v>8</v>
       </c>
       <c r="F52" t="s">
-        <v>17</v>
-      </c>
-      <c r="G52" t="s">
-        <v>18</v>
-      </c>
-      <c r="H52" s="59" t="s">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>1090</v>
+        <v>20</v>
+      </c>
+      <c r="H52" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" s="55" t="s">
+        <v>603</v>
       </c>
       <c r="B53" s="3">
-        <f>1000*$B$49*(Parameters!$B$5/7059)</f>
-        <v>3.901221594640746</v>
+        <f>6.9*$B$48*(Parameters!$B$5/7059)</f>
+        <v>2.691842900302115E-2</v>
       </c>
       <c r="C53" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" t="s">
+        <v>20</v>
+      </c>
+      <c r="H53" s="55" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>252</v>
+      </c>
+      <c r="B54" s="3">
+        <f>23.8*$B$48*(Parameters!$B$5/7059)</f>
+        <v>9.2849073952449762E-2</v>
+      </c>
+      <c r="C54" t="s">
         <v>558</v>
       </c>
-      <c r="D53" t="s">
-        <v>8</v>
-      </c>
-      <c r="F53" t="s">
-        <v>20</v>
-      </c>
-      <c r="H53" t="s">
-        <v>1091</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="55" t="s">
-        <v>603</v>
-      </c>
-      <c r="B54" s="3">
-        <f>6.9*$B$49*(Parameters!$B$5/7059)</f>
-        <v>2.691842900302115E-2</v>
-      </c>
-      <c r="C54" t="s">
-        <v>26</v>
-      </c>
       <c r="D54" t="s">
         <v>8</v>
       </c>
       <c r="F54" t="s">
         <v>20</v>
       </c>
-      <c r="H54" s="55" t="s">
-        <v>304</v>
+      <c r="H54" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B55" s="3">
-        <f>23.8*$B$49*(Parameters!$B$5/7059)</f>
-        <v>9.2849073952449762E-2</v>
+        <f>12.6*$B$48*(Parameters!$B$5/7059)</f>
+        <v>4.9155392092473403E-2</v>
       </c>
       <c r="C55" t="s">
         <v>558</v>
@@ -86318,19 +86339,19 @@
         <v>20</v>
       </c>
       <c r="H55" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>254</v>
+        <v>376</v>
       </c>
       <c r="B56" s="3">
-        <f>12.6*$B$49*(Parameters!$B$5/7059)</f>
-        <v>4.9155392092473403E-2</v>
+        <f>27*$B$48*(Parameters!$B$5/7059)</f>
+        <v>0.10533298305530014</v>
       </c>
       <c r="C56" t="s">
-        <v>558</v>
+        <v>26</v>
       </c>
       <c r="D56" t="s">
         <v>8</v>
@@ -86339,19 +86360,19 @@
         <v>20</v>
       </c>
       <c r="H56" t="s">
-        <v>256</v>
+        <v>377</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>376</v>
+        <v>626</v>
       </c>
       <c r="B57" s="3">
-        <f>27*$B$49*(Parameters!$B$5/7059)</f>
-        <v>0.10533298305530014</v>
+        <f>10.7*$B$48*(Parameters!$B$5/7059)</f>
+        <v>4.1743071062655977E-2</v>
       </c>
       <c r="C57" t="s">
-        <v>26</v>
+        <v>558</v>
       </c>
       <c r="D57" t="s">
         <v>8</v>
@@ -86360,16 +86381,16 @@
         <v>20</v>
       </c>
       <c r="H57" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>626</v>
+        <v>628</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A58" s="55" t="s">
+        <v>601</v>
       </c>
       <c r="B58" s="3">
-        <f>10.7*$B$49*(Parameters!$B$5/7059)</f>
-        <v>4.1743071062655977E-2</v>
+        <f>1.7*$B$48*(Parameters!$B$5/7059)</f>
+        <v>6.6320767108892682E-3</v>
       </c>
       <c r="C58" t="s">
         <v>558</v>
@@ -86380,20 +86401,20 @@
       <c r="F58" t="s">
         <v>20</v>
       </c>
-      <c r="H58" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="55" t="s">
-        <v>601</v>
+      <c r="H58" s="56" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>1081</v>
       </c>
       <c r="B59" s="3">
-        <f>1.7*$B$49*(Parameters!$B$5/7059)</f>
-        <v>6.6320767108892682E-3</v>
+        <f>(0.5+13.9)*$B$48*(Parameters!$B$5/7059)</f>
+        <v>5.6177590962826741E-2</v>
       </c>
       <c r="C59" t="s">
-        <v>558</v>
+        <v>26</v>
       </c>
       <c r="D59" t="s">
         <v>8</v>
@@ -86401,20 +86422,20 @@
       <c r="F59" t="s">
         <v>20</v>
       </c>
-      <c r="H59" s="56" t="s">
-        <v>602</v>
+      <c r="H59" t="s">
+        <v>1082</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>1081</v>
+        <v>338</v>
       </c>
       <c r="B60" s="3">
-        <f>(0.5+13.9)*$B$49*(Parameters!$B$5/7059)</f>
-        <v>5.6177590962826741E-2</v>
+        <f>1766*$B$48*(Parameters!$B$5/7059)</f>
+        <v>6.8895573361355575</v>
       </c>
       <c r="C60" t="s">
-        <v>26</v>
+        <v>610</v>
       </c>
       <c r="D60" t="s">
         <v>8</v>
@@ -86423,40 +86444,40 @@
         <v>20</v>
       </c>
       <c r="H60" t="s">
-        <v>1082</v>
+        <v>339</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>338</v>
+        <v>294</v>
       </c>
       <c r="B61" s="3">
-        <f>1766*$B$49*(Parameters!$B$5/7059)</f>
-        <v>6.8895573361355575</v>
+        <f>0.00000000822*$B$48*(Parameters!$B$5/7059)</f>
+        <v>3.2068041507946933E-11</v>
       </c>
       <c r="C61" t="s">
-        <v>610</v>
+        <v>26</v>
       </c>
       <c r="D61" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F61" t="s">
         <v>20</v>
       </c>
       <c r="H61" t="s">
-        <v>339</v>
+        <v>295</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>294</v>
+        <v>1084</v>
       </c>
       <c r="B62" s="3">
-        <f>0.00000000822*$B$49*(Parameters!$B$5/7059)</f>
-        <v>3.2068041507946933E-11</v>
+        <f>0.0000037*$B$48*(Parameters!$B$5/7059)</f>
+        <v>1.4434519900170761E-8</v>
       </c>
       <c r="C62" t="s">
-        <v>26</v>
+        <v>558</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>
@@ -86465,37 +86486,34 @@
         <v>20</v>
       </c>
       <c r="H62" t="s">
-        <v>295</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>1084</v>
+        <v>265</v>
       </c>
       <c r="B63" s="3">
-        <f>0.0000037*$B$49*(Parameters!$B$5/7059)</f>
-        <v>1.4434519900170761E-8</v>
-      </c>
-      <c r="C63" t="s">
-        <v>558</v>
+        <f>('Cavalett &amp; Cherubini 2022'!B52*'Cozzolini 2018'!$B$570)-Parameters!$B$15</f>
+        <v>5.1810216734533041</v>
       </c>
       <c r="D63" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E63" t="s">
+        <v>37</v>
       </c>
       <c r="F63" t="s">
-        <v>20</v>
-      </c>
-      <c r="H63" t="s">
-        <v>1084</v>
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>265</v>
-      </c>
-      <c r="B64" s="3">
-        <f>('Cavalett &amp; Cherubini 2022'!B53*'Cozzolini 2018'!$B$570)-Parameters!$B$15</f>
-        <v>5.1810216734533041</v>
+        <v>191</v>
+      </c>
+      <c r="B64" s="6">
+        <f>0.601*$B$48*(Parameters!$B$5/7059)</f>
+        <v>2.3446341783790884E-3</v>
       </c>
       <c r="D64" t="s">
         <v>8</v>
@@ -86509,11 +86527,11 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B65" s="6">
-        <f>0.601*$B$49*(Parameters!$B$5/7059)</f>
-        <v>2.3446341783790884E-3</v>
+        <f>0.3*$B$48*(Parameters!$B$5/7059)</f>
+        <v>1.1703664783922238E-3</v>
       </c>
       <c r="D65" t="s">
         <v>8</v>
@@ -86527,11 +86545,11 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>193</v>
+        <v>38</v>
       </c>
       <c r="B66" s="6">
-        <f>0.3*$B$49*(Parameters!$B$5/7059)</f>
-        <v>1.1703664783922238E-3</v>
+        <f>0.263*$B$48*(Parameters!$B$5/7059)</f>
+        <v>1.0260212793905162E-3</v>
       </c>
       <c r="D66" t="s">
         <v>8</v>
@@ -86545,11 +86563,11 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>38</v>
+        <v>314</v>
       </c>
       <c r="B67" s="6">
-        <f>0.263*$B$49*(Parameters!$B$5/7059)</f>
-        <v>1.0260212793905162E-3</v>
+        <f>0.00207*$B$48*(Parameters!$B$5/7059)</f>
+        <v>8.0755287009063426E-6</v>
       </c>
       <c r="D67" t="s">
         <v>8</v>
@@ -86563,11 +86581,11 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B68" s="6">
-        <f>0.00207*$B$49*(Parameters!$B$5/7059)</f>
-        <v>8.0755287009063426E-6</v>
+        <f>0.000563*$B$48*(Parameters!$B$5/7059)</f>
+        <v>2.19638775778274E-6</v>
       </c>
       <c r="D68" t="s">
         <v>8</v>
@@ -86581,11 +86599,11 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B69" s="6">
-        <f>0.000563*$B$49*(Parameters!$B$5/7059)</f>
-        <v>2.19638775778274E-6</v>
+        <f>0.0477*$B$48*(Parameters!$B$5/7059)</f>
+        <v>1.8608827006436358E-4</v>
       </c>
       <c r="D69" t="s">
         <v>8</v>
@@ -86599,11 +86617,11 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>312</v>
+        <v>40</v>
       </c>
       <c r="B70" s="6">
-        <f>0.0477*$B$49*(Parameters!$B$5/7059)</f>
-        <v>1.8608827006436358E-4</v>
+        <f>0.0271*$B$48*(Parameters!$B$5/7059)</f>
+        <v>1.0572310521476422E-4</v>
       </c>
       <c r="D70" t="s">
         <v>8</v>
@@ -86617,11 +86635,11 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>40</v>
+        <v>168</v>
       </c>
       <c r="B71" s="6">
-        <f>0.0271*$B$49*(Parameters!$B$5/7059)</f>
-        <v>1.0572310521476422E-4</v>
+        <f>0.0000903*$B$48*(Parameters!$B$5/7059)</f>
+        <v>3.5228030999605938E-7</v>
       </c>
       <c r="D71" t="s">
         <v>8</v>
@@ -86633,151 +86651,157 @@
         <v>36</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>168</v>
-      </c>
-      <c r="B72" s="6">
-        <f>0.0000903*$B$49*(Parameters!$B$5/7059)</f>
-        <v>3.5228030999605938E-7</v>
-      </c>
-      <c r="D72" t="s">
-        <v>8</v>
-      </c>
-      <c r="E72" t="s">
-        <v>37</v>
-      </c>
-      <c r="F72" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
+    <row r="73" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B74" s="58" t="s">
+      <c r="B73" s="58" t="s">
         <v>1092</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>2</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="B75" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>3</v>
-      </c>
-      <c r="B76" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="B76" s="67" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>4</v>
-      </c>
-      <c r="B77" s="67" t="s">
-        <v>1093</v>
+        <v>5</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>7</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>1110</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>9</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>1110</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B80" s="5"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>11</v>
+        <v>1087</v>
       </c>
       <c r="B81" s="5"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="B82" s="5"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>1088</v>
-      </c>
-      <c r="B83" s="5"/>
+        <v>485</v>
+      </c>
+      <c r="B83" s="66"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>485</v>
-      </c>
-      <c r="B84" s="66"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
         <v>1094</v>
       </c>
-      <c r="B85" s="28">
+      <c r="B84" s="28">
         <f>5728/(5728+1514+2524)</f>
         <v>0.58652467745238579</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
+    <row r="85" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B86" s="6"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B85" s="6"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>13</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C86" t="s">
+        <v>2</v>
+      </c>
+      <c r="D86" t="s">
+        <v>7</v>
+      </c>
+      <c r="E86" t="s">
+        <v>15</v>
+      </c>
+      <c r="F86" t="s">
+        <v>5</v>
+      </c>
+      <c r="G86" t="s">
+        <v>11</v>
+      </c>
+      <c r="H86" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>13</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>14</v>
+        <v>1092</v>
+      </c>
+      <c r="B87" s="3">
+        <v>1</v>
       </c>
       <c r="C87" t="s">
-        <v>2</v>
+        <v>558</v>
       </c>
       <c r="D87" t="s">
-        <v>7</v>
-      </c>
-      <c r="E87" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F87" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="G87" t="s">
-        <v>11</v>
-      </c>
-      <c r="H87" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="H87" s="67" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>1092</v>
+        <v>69</v>
       </c>
       <c r="B88" s="3">
-        <v>1</v>
+        <f>1000*$B$84*(Parameters!B6/5728)</f>
+        <v>3.8091337292647962</v>
       </c>
       <c r="C88" t="s">
         <v>558</v>
@@ -86786,22 +86810,19 @@
         <v>8</v>
       </c>
       <c r="F88" t="s">
-        <v>17</v>
-      </c>
-      <c r="G88" t="s">
-        <v>18</v>
-      </c>
-      <c r="H88" s="67" t="s">
-        <v>1093</v>
+        <v>20</v>
+      </c>
+      <c r="H88" s="6" t="s">
+        <v>851</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>69</v>
+        <v>252</v>
       </c>
       <c r="B89" s="3">
-        <f>1000*$B$85*(Parameters!B6/5728)</f>
-        <v>3.8091337292647962</v>
+        <f>1.8*$B$84*(Parameters!B6/5728)</f>
+        <v>6.8564407126766331E-3</v>
       </c>
       <c r="C89" t="s">
         <v>558</v>
@@ -86812,20 +86833,20 @@
       <c r="F89" t="s">
         <v>20</v>
       </c>
-      <c r="H89" s="6" t="s">
-        <v>851</v>
+      <c r="H89" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>252</v>
+        <v>376</v>
       </c>
       <c r="B90" s="3">
-        <f>1.8*$B$85*(Parameters!B6/5728)</f>
-        <v>6.8564407126766331E-3</v>
+        <f>0.45*$B$84*(Parameters!B6/5728)</f>
+        <v>1.7141101781691583E-3</v>
       </c>
       <c r="C90" t="s">
-        <v>558</v>
+        <v>26</v>
       </c>
       <c r="D90" t="s">
         <v>8</v>
@@ -86834,19 +86855,19 @@
         <v>20</v>
       </c>
       <c r="H90" t="s">
-        <v>253</v>
+        <v>377</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>376</v>
+        <v>338</v>
       </c>
       <c r="B91" s="3">
-        <f>0.45*$B$85*(Parameters!B6/5728)</f>
-        <v>1.7141101781691583E-3</v>
+        <f>77.2*$B$84*(Parameters!B6/5728)</f>
+        <v>0.29406512389924228</v>
       </c>
       <c r="C91" t="s">
-        <v>26</v>
+        <v>610</v>
       </c>
       <c r="D91" t="s">
         <v>8</v>
@@ -86855,19 +86876,19 @@
         <v>20</v>
       </c>
       <c r="H91" t="s">
-        <v>377</v>
+        <v>339</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>338</v>
+        <v>669</v>
       </c>
       <c r="B92" s="3">
-        <f>77.2*$B$85*(Parameters!B6/5728)</f>
-        <v>0.29406512389924228</v>
+        <f>5.5*$B$84*(Parameters!B6/5728)</f>
+        <v>2.0950235510956379E-2</v>
       </c>
       <c r="C92" t="s">
-        <v>610</v>
+        <v>31</v>
       </c>
       <c r="D92" t="s">
         <v>8</v>
@@ -86876,19 +86897,19 @@
         <v>20</v>
       </c>
       <c r="H92" t="s">
-        <v>339</v>
+        <v>670</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>669</v>
+        <v>1095</v>
       </c>
       <c r="B93" s="3">
-        <f>5.5*$B$85*(Parameters!B6/5728)</f>
-        <v>2.0950235510956379E-2</v>
+        <f>1.1*$B$84*(Parameters!B6/5728)</f>
+        <v>4.190047102191276E-3</v>
       </c>
       <c r="C93" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D93" t="s">
         <v>8</v>
@@ -86897,16 +86918,16 @@
         <v>20</v>
       </c>
       <c r="H93" t="s">
-        <v>670</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>1095</v>
+        <v>1097</v>
       </c>
       <c r="B94" s="3">
-        <f>1.1*$B$85*(Parameters!B6/5728)</f>
-        <v>4.190047102191276E-3</v>
+        <f>6.8*$B$84*(Parameters!B6/5728)</f>
+        <v>2.5902109359000614E-2</v>
       </c>
       <c r="C94" t="s">
         <v>26</v>
@@ -86918,37 +86939,37 @@
         <v>20</v>
       </c>
       <c r="H94" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>1097</v>
+        <v>1099</v>
       </c>
       <c r="B95" s="3">
-        <f>6.8*$B$85*(Parameters!B6/5728)</f>
-        <v>2.5902109359000614E-2</v>
+        <f>0.00000102*$B$84*(Parameters!B6/5728)</f>
+        <v>3.885316403850092E-9</v>
       </c>
       <c r="C95" t="s">
         <v>26</v>
       </c>
       <c r="D95" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F95" t="s">
         <v>20</v>
       </c>
       <c r="H95" t="s">
-        <v>1098</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>1099</v>
+        <v>1101</v>
       </c>
       <c r="B96" s="3">
-        <f>0.00000102*$B$85*(Parameters!B6/5728)</f>
-        <v>3.885316403850092E-9</v>
+        <f>0.000000503*$B$84*(Parameters!B6/5728)</f>
+        <v>1.9159942658201922E-9</v>
       </c>
       <c r="C96" t="s">
         <v>26</v>
@@ -86960,37 +86981,34 @@
         <v>20</v>
       </c>
       <c r="H96" t="s">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>1101</v>
+        <v>265</v>
       </c>
       <c r="B97" s="3">
-        <f>0.000000503*$B$85*(Parameters!B6/5728)</f>
-        <v>1.9159942658201922E-9</v>
-      </c>
-      <c r="C97" t="s">
-        <v>26</v>
+        <f>('Cavalett &amp; Cherubini 2022'!B88*'Cozzolini 2018'!$B$570)-Parameters!$B$16</f>
+        <v>4.0775445422895764</v>
       </c>
       <c r="D97" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E97" t="s">
+        <v>37</v>
       </c>
       <c r="F97" t="s">
-        <v>20</v>
-      </c>
-      <c r="H97" t="s">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>265</v>
-      </c>
-      <c r="B98" s="3">
-        <f>('Cavalett &amp; Cherubini 2022'!B89*'Cozzolini 2018'!$B$570)-Parameters!$B$16</f>
-        <v>4.0775445422895764</v>
+        <v>191</v>
+      </c>
+      <c r="B98" s="6">
+        <f>0.000441*$B$84*(Parameters!B6/5728)</f>
+        <v>1.6798279746057751E-6</v>
       </c>
       <c r="D98" t="s">
         <v>8</v>
@@ -87002,13 +87020,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B99" s="6">
-        <f>0.000441*$B$85*(Parameters!B6/5728)</f>
-        <v>1.6798279746057751E-6</v>
+        <f>0.00042*$B$84*(Parameters!B6/5728)</f>
+        <v>1.5998361662912144E-6</v>
       </c>
       <c r="D99" t="s">
         <v>8</v>
@@ -87020,13 +87038,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>193</v>
+        <v>38</v>
       </c>
       <c r="B100" s="6">
-        <f>0.00042*$B$85*(Parameters!B6/5728)</f>
-        <v>1.5998361662912144E-6</v>
+        <f>0.00376*$B$84*(Parameters!B6/5728)</f>
+        <v>1.4322342822035634E-5</v>
       </c>
       <c r="D100" t="s">
         <v>8</v>
@@ -87038,13 +87056,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>38</v>
+        <v>314</v>
       </c>
       <c r="B101" s="6">
-        <f>0.00376*$B$85*(Parameters!B6/5728)</f>
-        <v>1.4322342822035634E-5</v>
+        <f>0.000115*$B$84*(Parameters!B6/5728)</f>
+        <v>4.3805037886545155E-7</v>
       </c>
       <c r="D101" t="s">
         <v>8</v>
@@ -87056,13 +87074,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B102" s="6">
-        <f>0.000115*$B$85*(Parameters!B6/5728)</f>
-        <v>4.3805037886545155E-7</v>
+        <f>0.000042*$B$84*(Parameters!B6/5728)</f>
+        <v>1.5998361662912143E-7</v>
       </c>
       <c r="D102" t="s">
         <v>8</v>
@@ -87074,13 +87092,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>315</v>
+        <v>40</v>
       </c>
       <c r="B103" s="6">
-        <f>0.000042*$B$85*(Parameters!B6/5728)</f>
-        <v>1.5998361662912143E-7</v>
+        <f>0.000021*$B$84*(Parameters!B6/5728)</f>
+        <v>7.9991808314560717E-8</v>
       </c>
       <c r="D103" t="s">
         <v>8</v>
@@ -87092,151 +87110,157 @@
         <v>36</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>40</v>
-      </c>
-      <c r="B104" s="6">
-        <f>0.000021*$B$85*(Parameters!B6/5728)</f>
-        <v>7.9991808314560717E-8</v>
-      </c>
-      <c r="D104" t="s">
-        <v>8</v>
-      </c>
-      <c r="E104" t="s">
-        <v>37</v>
-      </c>
-      <c r="F104" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A106" s="1" t="s">
+    <row r="105" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B106" s="58" t="s">
+      <c r="B105" s="58" t="s">
         <v>1112</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>2</v>
-      </c>
-      <c r="B107" s="6" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="B107" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>3</v>
-      </c>
-      <c r="B108" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="B108" s="67" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>4</v>
-      </c>
-      <c r="B109" s="67" t="s">
-        <v>1093</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>7</v>
-      </c>
-      <c r="B111" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>9</v>
-      </c>
-      <c r="B112" s="6" t="s">
-        <v>1110</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B112" s="5"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>11</v>
+        <v>1087</v>
       </c>
       <c r="B113" s="5"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="B114" s="5"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>1088</v>
-      </c>
-      <c r="B115" s="5"/>
+        <v>485</v>
+      </c>
+      <c r="B115" s="66"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>485</v>
-      </c>
-      <c r="B116" s="66"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
         <v>1094</v>
       </c>
-      <c r="B117" s="28">
+      <c r="B116" s="28">
         <f>5728/(5728+1514+2524)</f>
         <v>0.58652467745238579</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A118" s="1" t="s">
+    <row r="117" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B118" s="6"/>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B117" s="6"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>13</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C118" t="s">
+        <v>2</v>
+      </c>
+      <c r="D118" t="s">
+        <v>7</v>
+      </c>
+      <c r="E118" t="s">
+        <v>15</v>
+      </c>
+      <c r="F118" t="s">
+        <v>5</v>
+      </c>
+      <c r="G118" t="s">
+        <v>11</v>
+      </c>
+      <c r="H118" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>13</v>
-      </c>
-      <c r="B119" s="6" t="s">
-        <v>14</v>
+        <v>1092</v>
+      </c>
+      <c r="B119" s="3">
+        <v>1</v>
       </c>
       <c r="C119" t="s">
-        <v>2</v>
+        <v>558</v>
       </c>
       <c r="D119" t="s">
-        <v>7</v>
-      </c>
-      <c r="E119" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F119" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="G119" t="s">
-        <v>11</v>
-      </c>
-      <c r="H119" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="H119" s="67" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="B120" s="3">
-        <v>1</v>
+        <f>1000*$B$116*(Parameters!B6/5728)</f>
+        <v>3.8091337292647962</v>
       </c>
       <c r="C120" t="s">
         <v>558</v>
@@ -87245,22 +87269,19 @@
         <v>8</v>
       </c>
       <c r="F120" t="s">
-        <v>17</v>
-      </c>
-      <c r="G120" t="s">
-        <v>18</v>
-      </c>
-      <c r="H120" s="67" t="s">
-        <v>1093</v>
+        <v>20</v>
+      </c>
+      <c r="H120" t="s">
+        <v>1091</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>1090</v>
+        <v>252</v>
       </c>
       <c r="B121" s="3">
-        <f>1000*$B$117*(Parameters!B6/5728)</f>
-        <v>3.8091337292647962</v>
+        <f>1.8*$B$116*(Parameters!B6/5728)</f>
+        <v>6.8564407126766331E-3</v>
       </c>
       <c r="C121" t="s">
         <v>558</v>
@@ -87272,19 +87293,19 @@
         <v>20</v>
       </c>
       <c r="H121" t="s">
-        <v>1091</v>
+        <v>253</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>252</v>
+        <v>376</v>
       </c>
       <c r="B122" s="3">
-        <f>1.8*$B$117*(Parameters!B6/5728)</f>
-        <v>6.8564407126766331E-3</v>
+        <f>0.45*$B$116*(Parameters!B6/5728)</f>
+        <v>1.7141101781691583E-3</v>
       </c>
       <c r="C122" t="s">
-        <v>558</v>
+        <v>26</v>
       </c>
       <c r="D122" t="s">
         <v>8</v>
@@ -87293,19 +87314,19 @@
         <v>20</v>
       </c>
       <c r="H122" t="s">
-        <v>253</v>
+        <v>377</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>376</v>
+        <v>338</v>
       </c>
       <c r="B123" s="3">
-        <f>0.45*$B$117*(Parameters!B6/5728)</f>
-        <v>1.7141101781691583E-3</v>
+        <f>77.2*$B$116*(Parameters!B6/5728)</f>
+        <v>0.29406512389924228</v>
       </c>
       <c r="C123" t="s">
-        <v>26</v>
+        <v>610</v>
       </c>
       <c r="D123" t="s">
         <v>8</v>
@@ -87314,19 +87335,19 @@
         <v>20</v>
       </c>
       <c r="H123" t="s">
-        <v>377</v>
+        <v>339</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>338</v>
+        <v>669</v>
       </c>
       <c r="B124" s="3">
-        <f>77.2*$B$117*(Parameters!B6/5728)</f>
-        <v>0.29406512389924228</v>
+        <f>5.5*$B$116*(Parameters!B6/5728)</f>
+        <v>2.0950235510956379E-2</v>
       </c>
       <c r="C124" t="s">
-        <v>610</v>
+        <v>31</v>
       </c>
       <c r="D124" t="s">
         <v>8</v>
@@ -87335,19 +87356,19 @@
         <v>20</v>
       </c>
       <c r="H124" t="s">
-        <v>339</v>
+        <v>670</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>669</v>
+        <v>1095</v>
       </c>
       <c r="B125" s="3">
-        <f>5.5*$B$117*(Parameters!B6/5728)</f>
-        <v>2.0950235510956379E-2</v>
+        <f>1.1*$B$116*(Parameters!B6/5728)</f>
+        <v>4.190047102191276E-3</v>
       </c>
       <c r="C125" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D125" t="s">
         <v>8</v>
@@ -87356,16 +87377,16 @@
         <v>20</v>
       </c>
       <c r="H125" t="s">
-        <v>670</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>1095</v>
+        <v>1097</v>
       </c>
       <c r="B126" s="3">
-        <f>1.1*$B$117*(Parameters!B6/5728)</f>
-        <v>4.190047102191276E-3</v>
+        <f>6.8*$B$116*(Parameters!B6/5728)</f>
+        <v>2.5902109359000614E-2</v>
       </c>
       <c r="C126" t="s">
         <v>26</v>
@@ -87377,37 +87398,37 @@
         <v>20</v>
       </c>
       <c r="H126" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>1097</v>
+        <v>1099</v>
       </c>
       <c r="B127" s="3">
-        <f>6.8*$B$117*(Parameters!B6/5728)</f>
-        <v>2.5902109359000614E-2</v>
+        <f>0.00000102*$B$116*(Parameters!B6/5728)</f>
+        <v>3.885316403850092E-9</v>
       </c>
       <c r="C127" t="s">
         <v>26</v>
       </c>
       <c r="D127" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F127" t="s">
         <v>20</v>
       </c>
       <c r="H127" t="s">
-        <v>1098</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>1099</v>
+        <v>1101</v>
       </c>
       <c r="B128" s="3">
-        <f>0.00000102*$B$117*(Parameters!B6/5728)</f>
-        <v>3.885316403850092E-9</v>
+        <f>0.000000503*$B$116*(Parameters!B6/5728)</f>
+        <v>1.9159942658201922E-9</v>
       </c>
       <c r="C128" t="s">
         <v>26</v>
@@ -87419,37 +87440,34 @@
         <v>20</v>
       </c>
       <c r="H128" t="s">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>1101</v>
+        <v>265</v>
       </c>
       <c r="B129" s="3">
-        <f>0.000000503*$B$117*(Parameters!B6/5728)</f>
-        <v>1.9159942658201922E-9</v>
-      </c>
-      <c r="C129" t="s">
-        <v>26</v>
+        <f>('Cavalett &amp; Cherubini 2022'!B120*'Cozzolini 2018'!$B$570)-Parameters!$B$16</f>
+        <v>4.0775445422895764</v>
       </c>
       <c r="D129" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E129" t="s">
+        <v>37</v>
       </c>
       <c r="F129" t="s">
-        <v>20</v>
-      </c>
-      <c r="H129" t="s">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>265</v>
-      </c>
-      <c r="B130" s="3">
-        <f>('Cavalett &amp; Cherubini 2022'!B121*'Cozzolini 2018'!$B$570)-Parameters!$B$16</f>
-        <v>4.0775445422895764</v>
+        <v>191</v>
+      </c>
+      <c r="B130" s="6">
+        <f>0.000441*$B$116*(Parameters!B6/5728)</f>
+        <v>1.6798279746057751E-6</v>
       </c>
       <c r="D130" t="s">
         <v>8</v>
@@ -87461,13 +87479,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B131" s="6">
-        <f>0.000441*$B$117*(Parameters!B6/5728)</f>
-        <v>1.6798279746057751E-6</v>
+        <f>0.00042*$B$116*(Parameters!B6/5728)</f>
+        <v>1.5998361662912144E-6</v>
       </c>
       <c r="D131" t="s">
         <v>8</v>
@@ -87479,13 +87497,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>193</v>
+        <v>38</v>
       </c>
       <c r="B132" s="6">
-        <f>0.00042*$B$117*(Parameters!B6/5728)</f>
-        <v>1.5998361662912144E-6</v>
+        <f>0.00376*$B$116*(Parameters!B6/5728)</f>
+        <v>1.4322342822035634E-5</v>
       </c>
       <c r="D132" t="s">
         <v>8</v>
@@ -87497,13 +87515,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>38</v>
+        <v>314</v>
       </c>
       <c r="B133" s="6">
-        <f>0.00376*$B$117*(Parameters!B6/5728)</f>
-        <v>1.4322342822035634E-5</v>
+        <f>0.000115*$B$116*(Parameters!B6/5728)</f>
+        <v>4.3805037886545155E-7</v>
       </c>
       <c r="D133" t="s">
         <v>8</v>
@@ -87515,13 +87533,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B134" s="6">
-        <f>0.000115*$B$117*(Parameters!B6/5728)</f>
-        <v>4.3805037886545155E-7</v>
+        <f>0.000042*$B$116*(Parameters!B6/5728)</f>
+        <v>1.5998361662912143E-7</v>
       </c>
       <c r="D134" t="s">
         <v>8</v>
@@ -87533,13 +87551,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>315</v>
+        <v>40</v>
       </c>
       <c r="B135" s="6">
-        <f>0.000042*$B$117*(Parameters!B6/5728)</f>
-        <v>1.5998361662912143E-7</v>
+        <f>0.000021*$B$116*(Parameters!B6/5728)</f>
+        <v>7.9991808314560717E-8</v>
       </c>
       <c r="D135" t="s">
         <v>8</v>
@@ -87551,153 +87569,159 @@
         <v>36</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
-        <v>40</v>
-      </c>
-      <c r="B136" s="6">
-        <f>0.000021*$B$117*(Parameters!B6/5728)</f>
-        <v>7.9991808314560717E-8</v>
-      </c>
-      <c r="D136" t="s">
-        <v>8</v>
-      </c>
-      <c r="E136" t="s">
-        <v>37</v>
-      </c>
-      <c r="F136" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A139" s="1" t="s">
+    <row r="138" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B139" s="58" t="s">
+      <c r="B138" s="58" t="s">
         <v>1104</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>2</v>
+      </c>
+      <c r="B139" s="6" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>2</v>
-      </c>
-      <c r="B140" s="6" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="B140" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>3</v>
-      </c>
-      <c r="B141" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="B141" s="67" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>4</v>
-      </c>
-      <c r="B142" s="67" t="s">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>7</v>
-      </c>
-      <c r="B144" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="B144" s="6" t="s">
+        <v>1110</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>9</v>
-      </c>
-      <c r="B145" s="6" t="s">
-        <v>1110</v>
+        <v>11</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>1109</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>11</v>
-      </c>
-      <c r="B146" s="5" t="s">
-        <v>1109</v>
-      </c>
+        <v>1087</v>
+      </c>
+      <c r="B146" s="5"/>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="B147" s="5"/>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>1088</v>
-      </c>
-      <c r="B148" s="5"/>
+        <v>485</v>
+      </c>
+      <c r="B148" s="66"/>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>485</v>
-      </c>
-      <c r="B149" s="66"/>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
         <v>1106</v>
       </c>
-      <c r="B150" s="28">
+      <c r="B149" s="28">
         <f>2524/(5728+1514+2524)</f>
         <v>0.25844767560925658</v>
       </c>
     </row>
-    <row r="151" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A151" s="1" t="s">
+    <row r="150" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A150" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B151" s="6"/>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B150" s="6"/>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>13</v>
+      </c>
+      <c r="B151" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C151" t="s">
+        <v>2</v>
+      </c>
+      <c r="D151" t="s">
+        <v>7</v>
+      </c>
+      <c r="E151" t="s">
+        <v>15</v>
+      </c>
+      <c r="F151" t="s">
+        <v>5</v>
+      </c>
+      <c r="G151" t="s">
+        <v>11</v>
+      </c>
+      <c r="H151" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>13</v>
-      </c>
-      <c r="B152" s="6" t="s">
-        <v>14</v>
+        <v>1104</v>
+      </c>
+      <c r="B152" s="3">
+        <v>1</v>
       </c>
       <c r="C152" t="s">
-        <v>2</v>
+        <v>558</v>
       </c>
       <c r="D152" t="s">
-        <v>7</v>
-      </c>
-      <c r="E152" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F152" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="G152" t="s">
-        <v>11</v>
-      </c>
-      <c r="H152" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="H152" s="67" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>1104</v>
+        <v>69</v>
       </c>
       <c r="B153" s="3">
-        <v>1</v>
+        <f>1000*$B$149*(Parameters!B7/5728)</f>
+        <v>1.9401623692733996</v>
       </c>
       <c r="C153" t="s">
         <v>558</v>
@@ -87706,22 +87730,19 @@
         <v>8</v>
       </c>
       <c r="F153" t="s">
-        <v>17</v>
-      </c>
-      <c r="G153" t="s">
-        <v>18</v>
-      </c>
-      <c r="H153" s="67" t="s">
-        <v>1105</v>
+        <v>20</v>
+      </c>
+      <c r="H153" s="6" t="s">
+        <v>851</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>69</v>
+        <v>252</v>
       </c>
       <c r="B154" s="3">
-        <f>1000*$B$150*(Parameters!B7/5728)</f>
-        <v>1.9401623692733996</v>
+        <f>1.8*$B$149*(Parameters!B7/5728)</f>
+        <v>3.4922922646921191E-3</v>
       </c>
       <c r="C154" t="s">
         <v>558</v>
@@ -87732,20 +87753,20 @@
       <c r="F154" t="s">
         <v>20</v>
       </c>
-      <c r="H154" s="6" t="s">
-        <v>851</v>
+      <c r="H154" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>252</v>
+        <v>376</v>
       </c>
       <c r="B155" s="3">
-        <f>1.8*$B$150*(Parameters!B7/5728)</f>
-        <v>3.4922922646921191E-3</v>
+        <f>0.45*$B$149*(Parameters!B7/5728)</f>
+        <v>8.7307306617302976E-4</v>
       </c>
       <c r="C155" t="s">
-        <v>558</v>
+        <v>26</v>
       </c>
       <c r="D155" t="s">
         <v>8</v>
@@ -87754,19 +87775,19 @@
         <v>20</v>
       </c>
       <c r="H155" t="s">
-        <v>253</v>
+        <v>377</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>376</v>
+        <v>338</v>
       </c>
       <c r="B156" s="3">
-        <f>0.45*$B$150*(Parameters!B7/5728)</f>
-        <v>8.7307306617302976E-4</v>
+        <f>77.2*$B$149*(Parameters!B7/5728)</f>
+        <v>0.14978053490790647</v>
       </c>
       <c r="C156" t="s">
-        <v>26</v>
+        <v>610</v>
       </c>
       <c r="D156" t="s">
         <v>8</v>
@@ -87775,19 +87796,19 @@
         <v>20</v>
       </c>
       <c r="H156" t="s">
-        <v>377</v>
+        <v>339</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>338</v>
+        <v>669</v>
       </c>
       <c r="B157" s="3">
-        <f>77.2*$B$150*(Parameters!B7/5728)</f>
-        <v>0.14978053490790647</v>
+        <f>5.5*$B$149*(Parameters!B7/5728)</f>
+        <v>1.0670893031003697E-2</v>
       </c>
       <c r="C157" t="s">
-        <v>610</v>
+        <v>31</v>
       </c>
       <c r="D157" t="s">
         <v>8</v>
@@ -87796,19 +87817,19 @@
         <v>20</v>
       </c>
       <c r="H157" t="s">
-        <v>339</v>
+        <v>670</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>669</v>
+        <v>1095</v>
       </c>
       <c r="B158" s="3">
-        <f>5.5*$B$150*(Parameters!B7/5728)</f>
-        <v>1.0670893031003697E-2</v>
+        <f>1.1*$B$149*(Parameters!B7/5728)</f>
+        <v>2.1341786062007398E-3</v>
       </c>
       <c r="C158" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D158" t="s">
         <v>8</v>
@@ -87817,16 +87838,16 @@
         <v>20</v>
       </c>
       <c r="H158" t="s">
-        <v>670</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>1095</v>
+        <v>1097</v>
       </c>
       <c r="B159" s="3">
-        <f>1.1*$B$150*(Parameters!B7/5728)</f>
-        <v>2.1341786062007398E-3</v>
+        <f>6.8*$B$149*(Parameters!B7/5728)</f>
+        <v>1.3193104111059116E-2</v>
       </c>
       <c r="C159" t="s">
         <v>26</v>
@@ -87838,37 +87859,37 @@
         <v>20</v>
       </c>
       <c r="H159" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>1097</v>
+        <v>1099</v>
       </c>
       <c r="B160" s="3">
-        <f>6.8*$B$150*(Parameters!B7/5728)</f>
-        <v>1.3193104111059116E-2</v>
+        <f>0.00000102*$B$149*(Parameters!B7/5728)</f>
+        <v>1.9789656166588675E-9</v>
       </c>
       <c r="C160" t="s">
         <v>26</v>
       </c>
       <c r="D160" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F160" t="s">
         <v>20</v>
       </c>
       <c r="H160" t="s">
-        <v>1098</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>1099</v>
+        <v>1101</v>
       </c>
       <c r="B161" s="3">
-        <f>0.00000102*$B$150*(Parameters!B7/5728)</f>
-        <v>1.9789656166588675E-9</v>
+        <f>0.000000503*$B$149*(Parameters!B7/5728)</f>
+        <v>9.7590167174451989E-10</v>
       </c>
       <c r="C161" t="s">
         <v>26</v>
@@ -87880,37 +87901,34 @@
         <v>20</v>
       </c>
       <c r="H161" t="s">
-        <v>1100</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>1101</v>
+        <v>265</v>
       </c>
       <c r="B162" s="3">
-        <f>0.000000503*$B$150*(Parameters!B7/5728)</f>
-        <v>9.7590167174451989E-10</v>
-      </c>
-      <c r="C162" t="s">
-        <v>26</v>
+        <f>('Cavalett &amp; Cherubini 2022'!B153*'Cozzolini 2018'!$B$570)-Parameters!$B$17</f>
+        <v>0.37850862891855597</v>
       </c>
       <c r="D162" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E162" t="s">
+        <v>37</v>
       </c>
       <c r="F162" t="s">
-        <v>20</v>
-      </c>
-      <c r="H162" t="s">
-        <v>1102</v>
+        <v>36</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>265</v>
-      </c>
-      <c r="B163" s="3">
-        <f>('Cavalett &amp; Cherubini 2022'!B154*'Cozzolini 2018'!$B$570)-Parameters!$B$17</f>
-        <v>0.37850862891855597</v>
+        <v>191</v>
+      </c>
+      <c r="B163" s="6">
+        <f>0.000441*$B$149*(Parameters!B7/5728)</f>
+        <v>8.5561160484956925E-7</v>
       </c>
       <c r="D163" t="s">
         <v>8</v>
@@ -87924,11 +87942,11 @@
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B164" s="6">
-        <f>0.000441*$B$150*(Parameters!B7/5728)</f>
-        <v>8.5561160484956925E-7</v>
+        <f>0.00042*$B$149*(Parameters!B7/5728)</f>
+        <v>8.1486819509482783E-7</v>
       </c>
       <c r="D164" t="s">
         <v>8</v>
@@ -87942,11 +87960,11 @@
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>193</v>
+        <v>38</v>
       </c>
       <c r="B165" s="6">
-        <f>0.00042*$B$150*(Parameters!B7/5728)</f>
-        <v>8.1486819509482783E-7</v>
+        <f>0.00376*$B$149*(Parameters!B7/5728)</f>
+        <v>7.2950105084679824E-6</v>
       </c>
       <c r="D165" t="s">
         <v>8</v>
@@ -87960,11 +87978,11 @@
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>38</v>
+        <v>314</v>
       </c>
       <c r="B166" s="6">
-        <f>0.00376*$B$150*(Parameters!B7/5728)</f>
-        <v>7.2950105084679824E-6</v>
+        <f>0.000115*$B$149*(Parameters!B7/5728)</f>
+        <v>2.2311867246644096E-7</v>
       </c>
       <c r="D166" t="s">
         <v>8</v>
@@ -87978,11 +87996,11 @@
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B167" s="6">
-        <f>0.000115*$B$150*(Parameters!B7/5728)</f>
-        <v>2.2311867246644096E-7</v>
+        <f>0.000042*$B$149*(Parameters!B7/5728)</f>
+        <v>8.1486819509482786E-8</v>
       </c>
       <c r="D167" t="s">
         <v>8</v>
@@ -87996,11 +88014,11 @@
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>315</v>
+        <v>40</v>
       </c>
       <c r="B168" s="6">
-        <f>0.000042*$B$150*(Parameters!B7/5728)</f>
-        <v>8.1486819509482786E-8</v>
+        <f>0.000021*$B$149*(Parameters!B7/5728)</f>
+        <v>4.0743409754741393E-8</v>
       </c>
       <c r="D168" t="s">
         <v>8</v>
@@ -88012,151 +88030,157 @@
         <v>36</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A169" t="s">
-        <v>40</v>
-      </c>
-      <c r="B169" s="6">
-        <f>0.000021*$B$150*(Parameters!B7/5728)</f>
-        <v>4.0743409754741393E-8</v>
-      </c>
-      <c r="D169" t="s">
-        <v>8</v>
-      </c>
-      <c r="E169" t="s">
-        <v>37</v>
-      </c>
-      <c r="F169" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A171" s="1" t="s">
+    <row r="170" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A170" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B171" s="58" t="s">
+      <c r="B170" s="58" t="s">
         <v>1108</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>2</v>
+      </c>
+      <c r="B171" s="6" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>2</v>
-      </c>
-      <c r="B172" s="6" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="B172" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>3</v>
-      </c>
-      <c r="B173" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="174" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="B173" s="67" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>4</v>
-      </c>
-      <c r="B174" s="67" t="s">
-        <v>1105</v>
+        <v>5</v>
+      </c>
+      <c r="B174" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>7</v>
-      </c>
-      <c r="B176" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="B176" s="6" t="s">
+        <v>1110</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>9</v>
-      </c>
-      <c r="B177" s="6" t="s">
-        <v>1110</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B177" s="5"/>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>11</v>
+        <v>1087</v>
       </c>
       <c r="B178" s="5"/>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="B179" s="5"/>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>1088</v>
-      </c>
-      <c r="B180" s="5"/>
+        <v>485</v>
+      </c>
+      <c r="B180" s="66"/>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>485</v>
-      </c>
-      <c r="B181" s="66"/>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A182" t="s">
         <v>1106</v>
       </c>
-      <c r="B182" s="28">
+      <c r="B181" s="28">
         <f>2524/(5728+1514+2524)</f>
         <v>0.25844767560925658</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A183" s="1" t="s">
+    <row r="182" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A182" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B183" s="6"/>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B182" s="6"/>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>13</v>
+      </c>
+      <c r="B183" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C183" t="s">
+        <v>2</v>
+      </c>
+      <c r="D183" t="s">
+        <v>7</v>
+      </c>
+      <c r="E183" t="s">
+        <v>15</v>
+      </c>
+      <c r="F183" t="s">
+        <v>5</v>
+      </c>
+      <c r="G183" t="s">
+        <v>11</v>
+      </c>
+      <c r="H183" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>13</v>
-      </c>
-      <c r="B184" s="6" t="s">
-        <v>14</v>
+        <v>1108</v>
+      </c>
+      <c r="B184" s="3">
+        <v>1</v>
       </c>
       <c r="C184" t="s">
-        <v>2</v>
+        <v>558</v>
       </c>
       <c r="D184" t="s">
-        <v>7</v>
-      </c>
-      <c r="E184" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F184" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="G184" t="s">
-        <v>11</v>
-      </c>
-      <c r="H184" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="185" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="H184" s="67" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>1108</v>
+        <v>1090</v>
       </c>
       <c r="B185" s="3">
-        <v>1</v>
+        <f>1000*$B$181*(Parameters!B7/5728)</f>
+        <v>1.9401623692733996</v>
       </c>
       <c r="C185" t="s">
         <v>558</v>
@@ -88165,22 +88189,19 @@
         <v>8</v>
       </c>
       <c r="F185" t="s">
-        <v>17</v>
-      </c>
-      <c r="G185" t="s">
-        <v>18</v>
-      </c>
-      <c r="H185" s="67" t="s">
-        <v>1105</v>
+        <v>20</v>
+      </c>
+      <c r="H185" s="6" t="s">
+        <v>1091</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>1090</v>
+        <v>252</v>
       </c>
       <c r="B186" s="3">
-        <f>1000*$B$182*(Parameters!B7/5728)</f>
-        <v>1.9401623692733996</v>
+        <f>1.8*$B$181*(Parameters!B7/5728)</f>
+        <v>3.4922922646921191E-3</v>
       </c>
       <c r="C186" t="s">
         <v>558</v>
@@ -88191,20 +88212,20 @@
       <c r="F186" t="s">
         <v>20</v>
       </c>
-      <c r="H186" s="6" t="s">
-        <v>1091</v>
+      <c r="H186" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>252</v>
+        <v>376</v>
       </c>
       <c r="B187" s="3">
-        <f>1.8*$B$182*(Parameters!B7/5728)</f>
-        <v>3.4922922646921191E-3</v>
+        <f>0.45*$B$181*(Parameters!B7/5728)</f>
+        <v>8.7307306617302976E-4</v>
       </c>
       <c r="C187" t="s">
-        <v>558</v>
+        <v>26</v>
       </c>
       <c r="D187" t="s">
         <v>8</v>
@@ -88213,19 +88234,19 @@
         <v>20</v>
       </c>
       <c r="H187" t="s">
-        <v>253</v>
+        <v>377</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>376</v>
+        <v>338</v>
       </c>
       <c r="B188" s="3">
-        <f>0.45*$B$182*(Parameters!B7/5728)</f>
-        <v>8.7307306617302976E-4</v>
+        <f>77.2*$B$181*(Parameters!B7/5728)</f>
+        <v>0.14978053490790647</v>
       </c>
       <c r="C188" t="s">
-        <v>26</v>
+        <v>610</v>
       </c>
       <c r="D188" t="s">
         <v>8</v>
@@ -88234,19 +88255,19 @@
         <v>20</v>
       </c>
       <c r="H188" t="s">
-        <v>377</v>
+        <v>339</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>338</v>
+        <v>669</v>
       </c>
       <c r="B189" s="3">
-        <f>77.2*$B$182*(Parameters!B7/5728)</f>
-        <v>0.14978053490790647</v>
+        <f>5.5*$B$181*(Parameters!B7/5728)</f>
+        <v>1.0670893031003697E-2</v>
       </c>
       <c r="C189" t="s">
-        <v>610</v>
+        <v>31</v>
       </c>
       <c r="D189" t="s">
         <v>8</v>
@@ -88255,19 +88276,19 @@
         <v>20</v>
       </c>
       <c r="H189" t="s">
-        <v>339</v>
+        <v>670</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>669</v>
+        <v>1095</v>
       </c>
       <c r="B190" s="3">
-        <f>5.5*$B$182*(Parameters!B7/5728)</f>
-        <v>1.0670893031003697E-2</v>
+        <f>1.1*$B$181*(Parameters!B7/5728)</f>
+        <v>2.1341786062007398E-3</v>
       </c>
       <c r="C190" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D190" t="s">
         <v>8</v>
@@ -88276,16 +88297,16 @@
         <v>20</v>
       </c>
       <c r="H190" t="s">
-        <v>670</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>1095</v>
+        <v>1097</v>
       </c>
       <c r="B191" s="3">
-        <f>1.1*$B$182*(Parameters!B7/5728)</f>
-        <v>2.1341786062007398E-3</v>
+        <f>6.8*$B$181*(Parameters!B7/5728)</f>
+        <v>1.3193104111059116E-2</v>
       </c>
       <c r="C191" t="s">
         <v>26</v>
@@ -88297,37 +88318,37 @@
         <v>20</v>
       </c>
       <c r="H191" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>1097</v>
+        <v>1099</v>
       </c>
       <c r="B192" s="3">
-        <f>6.8*$B$182*(Parameters!B7/5728)</f>
-        <v>1.3193104111059116E-2</v>
+        <f>0.00000102*$B$181*(Parameters!B7/5728)</f>
+        <v>1.9789656166588675E-9</v>
       </c>
       <c r="C192" t="s">
         <v>26</v>
       </c>
       <c r="D192" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F192" t="s">
         <v>20</v>
       </c>
       <c r="H192" t="s">
-        <v>1098</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>1099</v>
+        <v>1101</v>
       </c>
       <c r="B193" s="3">
-        <f>0.00000102*$B$182*(Parameters!B7/5728)</f>
-        <v>1.9789656166588675E-9</v>
+        <f>0.000000503*$B$181*(Parameters!B7/5728)</f>
+        <v>9.7590167174451989E-10</v>
       </c>
       <c r="C193" t="s">
         <v>26</v>
@@ -88339,37 +88360,34 @@
         <v>20</v>
       </c>
       <c r="H193" t="s">
-        <v>1100</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>1101</v>
+        <v>265</v>
       </c>
       <c r="B194" s="3">
-        <f>0.000000503*$B$182*(Parameters!B7/5728)</f>
-        <v>9.7590167174451989E-10</v>
-      </c>
-      <c r="C194" t="s">
-        <v>26</v>
+        <f>('Cavalett &amp; Cherubini 2022'!B185*'Cozzolini 2018'!$B$570)-Parameters!$B$17</f>
+        <v>0.37850862891855597</v>
       </c>
       <c r="D194" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E194" t="s">
+        <v>37</v>
       </c>
       <c r="F194" t="s">
-        <v>20</v>
-      </c>
-      <c r="H194" t="s">
-        <v>1102</v>
+        <v>36</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>265</v>
-      </c>
-      <c r="B195" s="3">
-        <f>('Cavalett &amp; Cherubini 2022'!B186*'Cozzolini 2018'!$B$570)-Parameters!$B$17</f>
-        <v>0.37850862891855597</v>
+        <v>191</v>
+      </c>
+      <c r="B195" s="6">
+        <f>0.000441*$B$181*(Parameters!B7/5728)</f>
+        <v>8.5561160484956925E-7</v>
       </c>
       <c r="D195" t="s">
         <v>8</v>
@@ -88383,11 +88401,11 @@
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B196" s="6">
-        <f>0.000441*$B$182*(Parameters!B7/5728)</f>
-        <v>8.5561160484956925E-7</v>
+        <f>0.00042*$B$181*(Parameters!B7/5728)</f>
+        <v>8.1486819509482783E-7</v>
       </c>
       <c r="D196" t="s">
         <v>8</v>
@@ -88401,11 +88419,11 @@
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>193</v>
+        <v>38</v>
       </c>
       <c r="B197" s="6">
-        <f>0.00042*$B$182*(Parameters!B7/5728)</f>
-        <v>8.1486819509482783E-7</v>
+        <f>0.00376*$B$181*(Parameters!B7/5728)</f>
+        <v>7.2950105084679824E-6</v>
       </c>
       <c r="D197" t="s">
         <v>8</v>
@@ -88419,11 +88437,11 @@
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>38</v>
+        <v>314</v>
       </c>
       <c r="B198" s="6">
-        <f>0.00376*$B$182*(Parameters!B7/5728)</f>
-        <v>7.2950105084679824E-6</v>
+        <f>0.000115*$B$181*(Parameters!B7/5728)</f>
+        <v>2.2311867246644096E-7</v>
       </c>
       <c r="D198" t="s">
         <v>8</v>
@@ -88437,11 +88455,11 @@
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B199" s="6">
-        <f>0.000115*$B$182*(Parameters!B7/5728)</f>
-        <v>2.2311867246644096E-7</v>
+        <f>0.000042*$B$181*(Parameters!B7/5728)</f>
+        <v>8.1486819509482786E-8</v>
       </c>
       <c r="D199" t="s">
         <v>8</v>
@@ -88455,11 +88473,11 @@
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>315</v>
+        <v>40</v>
       </c>
       <c r="B200" s="6">
-        <f>0.000042*$B$182*(Parameters!B7/5728)</f>
-        <v>8.1486819509482786E-8</v>
+        <f>0.000021*$B$181*(Parameters!B7/5728)</f>
+        <v>4.0743409754741393E-8</v>
       </c>
       <c r="D200" t="s">
         <v>8</v>
@@ -88471,26 +88489,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A201" t="s">
-        <v>40</v>
-      </c>
-      <c r="B201" s="6">
-        <f>0.000021*$B$182*(Parameters!B7/5728)</f>
-        <v>4.0743409754741393E-8</v>
-      </c>
-      <c r="D201" t="s">
-        <v>8</v>
-      </c>
-      <c r="E201" t="s">
-        <v>37</v>
-      </c>
-      <c r="F201" t="s">
-        <v>36</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:H201" xr:uid="{06F5820A-E001-4A42-8382-32FC181BB2BB}"/>
+  <autoFilter ref="A1:H200" xr:uid="{06F5820A-E001-4A42-8382-32FC181BB2BB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Fix CCS issue Align with TIAM branch
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-biofuels.xlsx
+++ b/premise/data/additional_inventories/lci-biofuels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04821D4F-9EAD-B642-A1A2-1C6CBA3790F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAF6AFB-80E7-4C45-89E5-969020993CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35060" yWindow="100" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -580,7 +580,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19313" uniqueCount="1150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19437" uniqueCount="1161">
   <si>
     <t>Database</t>
   </si>
@@ -4059,12 +4059,45 @@
   <si>
     <t>carbon dioxide storage at wood burning power plant 20 MW post, pipeline 200km, storage 1000m</t>
   </si>
+  <si>
+    <t>kerosene production, via Fischer-Tropsch, from forest product (non-residual), energy allocation</t>
+  </si>
+  <si>
+    <t>1.81kg CO2/kg wood chips. Kerosene: 3.15 kgCO2/kg</t>
+  </si>
+  <si>
+    <t>kerosene production, via Fischer-Tropsch, from forest product (non-residual), with carbon capture and storage, energy allocation</t>
+  </si>
+  <si>
+    <t>230 kWh/t CO2 liquefied</t>
+  </si>
+  <si>
+    <t>market for monoethanolamine</t>
+  </si>
+  <si>
+    <t>monoethanolamine</t>
+  </si>
+  <si>
+    <t>4 kg MEA/t CO2 captured</t>
+  </si>
+  <si>
+    <t>carbon dioxide compression, transport and storage</t>
+  </si>
+  <si>
+    <t>carbon dioxide, stored</t>
+  </si>
+  <si>
+    <t>90% of CO2 emissions</t>
+  </si>
+  <si>
+    <t>Unravelling the role of biofuels in road transport under rapid electrification. Otavio Cavalett, Francesco Cherubini, 2022. https://doi.org/10.1002/bbb.2395. CCS is assumed to capture 90% of CO2 emissions. We add an input of 4 kg MEA/t CO2 captured as well as 230 kWh/t CO2 for liquefaction, based on studies on CCS of MSWI plants (Bisinella et al, 2022). CO2 transport and storage is from Qiu et al., 2022..</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
@@ -4072,6 +4105,7 @@
     <numFmt numFmtId="168" formatCode="[$€-2]\ #,##0;[Red]\-[$€-2]\ #,##0"/>
     <numFmt numFmtId="169" formatCode="0.0"/>
     <numFmt numFmtId="170" formatCode="0.0%"/>
+    <numFmt numFmtId="173" formatCode="0.00000"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -4348,7 +4382,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4446,6 +4480,7 @@
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -7636,11 +7671,11 @@
       </c>
       <c r="F61" s="35">
         <f>'Cavalett &amp; Cherubini 2022'!B153</f>
-        <v>1.9401623692733996</v>
+        <v>4.4030309236125333</v>
       </c>
       <c r="G61" s="36">
         <f t="shared" si="12"/>
-        <v>36.863085016194589</v>
+        <v>83.657587548638134</v>
       </c>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
@@ -7652,18 +7687,18 @@
       </c>
       <c r="M61" s="5">
         <f>'Cavalett &amp; Cherubini 2022'!B162</f>
-        <v>0.37850862891855597</v>
+        <v>4.8194859717386862</v>
       </c>
       <c r="N61">
         <v>43</v>
       </c>
       <c r="O61" s="28">
         <f t="shared" si="10"/>
-        <v>1.1664786053882727</v>
+        <v>0.51400000000000001</v>
       </c>
       <c r="P61" s="28">
         <f t="shared" si="11"/>
-        <v>1.1664786053882727</v>
+        <v>0.51400000000000001</v>
       </c>
       <c r="Q61" s="36"/>
     </row>
@@ -7682,11 +7717,11 @@
       </c>
       <c r="F62" s="35">
         <f>'Cavalett &amp; Cherubini 2022'!B185</f>
-        <v>1.9401623692733996</v>
+        <v>4.4030309236125333</v>
       </c>
       <c r="G62" s="36">
         <f t="shared" si="12"/>
-        <v>36.863085016194589</v>
+        <v>83.657587548638134</v>
       </c>
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
@@ -7698,18 +7733,18 @@
       </c>
       <c r="M62" s="5">
         <f>'Cavalett &amp; Cherubini 2022'!B194</f>
-        <v>0.37850862891855597</v>
+        <v>4.8194859717386862</v>
       </c>
       <c r="N62">
         <v>43</v>
       </c>
       <c r="O62" s="28">
         <f t="shared" si="10"/>
-        <v>1.1664786053882727</v>
+        <v>0.51400000000000001</v>
       </c>
       <c r="P62" s="28">
         <f t="shared" si="11"/>
-        <v>1.1664786053882727</v>
+        <v>0.51400000000000001</v>
       </c>
       <c r="Q62" s="36"/>
     </row>
@@ -9387,11 +9422,11 @@
       </c>
       <c r="F94" s="5">
         <f t="shared" si="13"/>
-        <v>4.5120055099381384E-2</v>
+        <v>0.10239606799098915</v>
       </c>
       <c r="G94" s="5">
         <f t="shared" si="14"/>
-        <v>0.85728104688824625</v>
+        <v>1.9455252918287937</v>
       </c>
       <c r="H94" s="4">
         <f t="shared" si="15"/>
@@ -9415,7 +9450,7 @@
       </c>
       <c r="M94" s="4">
         <f t="shared" si="20"/>
-        <v>8.8025262539199057E-3</v>
+        <v>0.11208106911020201</v>
       </c>
       <c r="N94" s="35">
         <f t="shared" si="21"/>
@@ -9423,11 +9458,11 @@
       </c>
       <c r="O94" s="28">
         <f t="shared" si="27"/>
-        <v>1.1664786053882727</v>
+        <v>0.51400000000000001</v>
       </c>
       <c r="P94" s="28">
         <f t="shared" si="28"/>
-        <v>1.1664786053882727</v>
+        <v>0.51400000000000001</v>
       </c>
     </row>
     <row r="95" spans="2:16" ht="16" x14ac:dyDescent="0.2">
@@ -9445,11 +9480,11 @@
       </c>
       <c r="F95" s="5">
         <f t="shared" si="13"/>
-        <v>4.5120055099381384E-2</v>
+        <v>0.10239606799098915</v>
       </c>
       <c r="G95" s="5">
         <f t="shared" si="14"/>
-        <v>0.85728104688824625</v>
+        <v>1.9455252918287937</v>
       </c>
       <c r="H95" s="4">
         <f t="shared" si="15"/>
@@ -9473,7 +9508,7 @@
       </c>
       <c r="M95" s="4">
         <f t="shared" si="20"/>
-        <v>8.8025262539199057E-3</v>
+        <v>0.11208106911020201</v>
       </c>
       <c r="N95" s="35">
         <f t="shared" si="21"/>
@@ -9481,11 +9516,11 @@
       </c>
       <c r="O95" s="28">
         <f t="shared" si="27"/>
-        <v>1.1664786053882727</v>
+        <v>0.51400000000000001</v>
       </c>
       <c r="P95" s="28">
         <f t="shared" si="28"/>
-        <v>1.1664786053882727</v>
+        <v>0.51400000000000001</v>
       </c>
     </row>
     <row r="97" spans="2:17" ht="21" x14ac:dyDescent="0.25">
@@ -13496,8 +13531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J2872"/>
   <sheetViews>
-    <sheetView zoomScale="131" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="B2873" sqref="B2873"/>
+    <sheetView topLeftCell="A831" zoomScale="131" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="B838" sqref="B838"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -59310,7 +59345,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -59332,7 +59366,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -59340,7 +59374,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -59348,7 +59382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -59356,7 +59390,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -59364,7 +59398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -59372,7 +59406,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -59380,7 +59414,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -59388,7 +59422,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>827</v>
       </c>
@@ -59397,7 +59431,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1147</v>
       </c>
@@ -59406,7 +59440,7 @@
         <v>5.2920000000000007</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>833</v>
       </c>
@@ -59416,12 +59450,12 @@
       </c>
       <c r="D11" s="28"/>
     </row>
-    <row r="12" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -59447,7 +59481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>76</v>
       </c>
@@ -59470,7 +59504,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -59494,7 +59528,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -59518,7 +59552,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -59542,7 +59576,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -59566,7 +59600,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>105</v>
       </c>
@@ -59590,7 +59624,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -59614,7 +59648,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -59638,7 +59672,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>340</v>
       </c>
@@ -59662,7 +59696,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>305</v>
       </c>
@@ -59686,7 +59720,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>308</v>
       </c>
@@ -59710,7 +59744,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>310</v>
       </c>
@@ -59734,7 +59768,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>265</v>
       </c>
@@ -59755,7 +59789,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>315</v>
       </c>
@@ -59775,7 +59809,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>155</v>
       </c>
@@ -59795,7 +59829,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>316</v>
       </c>
@@ -59815,7 +59849,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -59835,7 +59869,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>193</v>
       </c>
@@ -59855,7 +59889,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>317</v>
       </c>
@@ -59875,7 +59909,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>318</v>
       </c>
@@ -59895,7 +59929,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>314</v>
       </c>
@@ -59915,7 +59949,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>200</v>
       </c>
@@ -59935,7 +59969,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>319</v>
       </c>
@@ -59955,7 +59989,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>313</v>
       </c>
@@ -59975,7 +60009,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>154</v>
       </c>
@@ -59995,7 +60029,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>198</v>
       </c>
@@ -60015,7 +60049,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>138</v>
       </c>
@@ -60035,7 +60069,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>191</v>
       </c>
@@ -60055,7 +60089,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>127</v>
       </c>
@@ -60075,7 +60109,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>173</v>
       </c>
@@ -60095,7 +60129,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>199</v>
       </c>
@@ -60115,7 +60149,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>312</v>
       </c>
@@ -60135,7 +60169,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>148</v>
       </c>
@@ -60155,7 +60189,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>168</v>
       </c>
@@ -60175,7 +60209,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>206</v>
       </c>
@@ -60195,7 +60229,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>145</v>
       </c>
@@ -60215,7 +60249,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>168</v>
       </c>
@@ -60235,7 +60269,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>38</v>
       </c>
@@ -60255,7 +60289,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>132</v>
       </c>
@@ -60275,7 +60309,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>320</v>
       </c>
@@ -60295,7 +60329,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>142</v>
       </c>
@@ -60315,7 +60349,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>1008</v>
       </c>
@@ -60335,7 +60369,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>202</v>
       </c>
@@ -60355,7 +60389,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>126</v>
       </c>
@@ -60375,7 +60409,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>108</v>
       </c>
@@ -60396,7 +60430,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>172</v>
       </c>
@@ -60416,7 +60450,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>321</v>
       </c>
@@ -60456,8 +60490,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="1:7" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>1</v>
       </c>
@@ -60465,7 +60498,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>2</v>
       </c>
@@ -60473,7 +60506,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>3</v>
       </c>
@@ -60481,7 +60514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>4</v>
       </c>
@@ -60489,7 +60522,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>5</v>
       </c>
@@ -60497,7 +60530,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -60505,7 +60538,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>9</v>
       </c>
@@ -60513,7 +60546,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>11</v>
       </c>
@@ -60521,7 +60554,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>827</v>
       </c>
@@ -60530,7 +60563,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>833</v>
       </c>
@@ -60539,12 +60572,12 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>13</v>
       </c>
@@ -60570,7 +60603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>266</v>
       </c>
@@ -60593,7 +60626,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>22</v>
       </c>
@@ -60617,7 +60650,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>54</v>
       </c>
@@ -60641,7 +60674,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>340</v>
       </c>
@@ -60665,7 +60698,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>1008</v>
       </c>
@@ -60686,7 +60719,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>108</v>
       </c>
@@ -60706,7 +60739,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>194</v>
       </c>
@@ -60726,7 +60759,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>195</v>
       </c>
@@ -60746,7 +60779,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>196</v>
       </c>
@@ -60786,8 +60819,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="86" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>1</v>
       </c>
@@ -60795,7 +60827,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>2</v>
       </c>
@@ -60803,7 +60835,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>3</v>
       </c>
@@ -60811,7 +60843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>4</v>
       </c>
@@ -60819,7 +60851,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>5</v>
       </c>
@@ -60827,7 +60859,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>7</v>
       </c>
@@ -60835,7 +60867,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>9</v>
       </c>
@@ -60843,7 +60875,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>11</v>
       </c>
@@ -60851,7 +60883,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>485</v>
       </c>
@@ -60860,12 +60892,12 @@
         <v>0.64283077198483141</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>13</v>
       </c>
@@ -60891,7 +60923,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>291</v>
       </c>
@@ -60914,7 +60946,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>266</v>
       </c>
@@ -60938,7 +60970,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>294</v>
       </c>
@@ -60962,7 +60994,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>288</v>
       </c>
@@ -60986,7 +61018,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>252</v>
       </c>
@@ -61010,7 +61042,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>297</v>
       </c>
@@ -61034,7 +61066,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>303</v>
       </c>
@@ -61058,7 +61090,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>254</v>
       </c>
@@ -61082,7 +61114,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>265</v>
       </c>
@@ -61103,7 +61135,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="70" t="s">
         <v>338</v>
       </c>
@@ -61125,8 +61157,7 @@
       </c>
       <c r="H106" s="2"/>
     </row>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="108" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>1</v>
       </c>
@@ -61134,7 +61165,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>2</v>
       </c>
@@ -61142,7 +61173,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>3</v>
       </c>
@@ -61150,7 +61181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>4</v>
       </c>
@@ -61158,7 +61189,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>5</v>
       </c>
@@ -61166,7 +61197,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>7</v>
       </c>
@@ -61174,7 +61205,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>9</v>
       </c>
@@ -61182,7 +61213,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>11</v>
       </c>
@@ -61190,7 +61221,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>485</v>
       </c>
@@ -61199,12 +61230,12 @@
         <v>0.55032625843716321</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>13</v>
       </c>
@@ -61230,7 +61261,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>323</v>
       </c>
@@ -61253,7 +61284,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>266</v>
       </c>
@@ -61277,7 +61308,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>294</v>
       </c>
@@ -61301,7 +61332,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>288</v>
       </c>
@@ -61325,7 +61356,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>252</v>
       </c>
@@ -61349,7 +61380,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>297</v>
       </c>
@@ -61373,7 +61404,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>303</v>
       </c>
@@ -61397,7 +61428,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>254</v>
       </c>
@@ -61421,7 +61452,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>265</v>
       </c>
@@ -61442,7 +61473,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="70" t="s">
         <v>338</v>
       </c>
@@ -61464,8 +61495,7 @@
       </c>
       <c r="H128" s="2"/>
     </row>
-    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="130" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>1</v>
       </c>
@@ -61473,7 +61503,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>2</v>
       </c>
@@ -61481,7 +61511,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>3</v>
       </c>
@@ -61489,7 +61519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>4</v>
       </c>
@@ -61497,7 +61527,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>5</v>
       </c>
@@ -61505,7 +61535,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>7</v>
       </c>
@@ -61513,7 +61543,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>9</v>
       </c>
@@ -61521,7 +61551,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>11</v>
       </c>
@@ -61529,7 +61559,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>485</v>
       </c>
@@ -61538,12 +61568,12 @@
         <v>0.47247814788566023</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>13</v>
       </c>
@@ -61569,7 +61599,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>524</v>
       </c>
@@ -61592,7 +61622,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>266</v>
       </c>
@@ -61616,7 +61646,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>294</v>
       </c>
@@ -61640,7 +61670,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>288</v>
       </c>
@@ -61664,7 +61694,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>252</v>
       </c>
@@ -61688,7 +61718,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>297</v>
       </c>
@@ -61712,7 +61742,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>303</v>
       </c>
@@ -61736,7 +61766,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>254</v>
       </c>
@@ -61760,7 +61790,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>265</v>
       </c>
@@ -61781,7 +61811,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="150" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>28</v>
       </c>
@@ -61805,7 +61835,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="151" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A151" s="70" t="s">
         <v>338</v>
       </c>
@@ -61827,8 +61857,7 @@
       </c>
       <c r="H151" s="2"/>
     </row>
-    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="153" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>1</v>
       </c>
@@ -61836,7 +61865,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>2</v>
       </c>
@@ -61844,7 +61873,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>3</v>
       </c>
@@ -61852,7 +61881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>4</v>
       </c>
@@ -61860,7 +61889,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>5</v>
       </c>
@@ -61868,7 +61897,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>7</v>
       </c>
@@ -61876,7 +61905,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>9</v>
       </c>
@@ -61884,7 +61913,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>11</v>
       </c>
@@ -61892,12 +61921,12 @@
         <v>350</v>
       </c>
     </row>
-    <row r="161" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>13</v>
       </c>
@@ -61929,7 +61958,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>346</v>
       </c>
@@ -61952,7 +61981,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="164" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>291</v>
       </c>
@@ -61975,7 +62004,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>28</v>
       </c>
@@ -61995,7 +62024,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>328</v>
       </c>
@@ -62015,7 +62044,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>330</v>
       </c>
@@ -62035,7 +62064,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>332</v>
       </c>
@@ -62055,7 +62084,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>334</v>
       </c>
@@ -62075,7 +62104,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>336</v>
       </c>
@@ -62095,7 +62124,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>338</v>
       </c>
@@ -62115,7 +62144,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>100</v>
       </c>
@@ -62135,7 +62164,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>340</v>
       </c>
@@ -62155,7 +62184,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>342</v>
       </c>
@@ -62175,8 +62204,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="175" spans="1:10" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="176" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>1</v>
       </c>
@@ -62184,7 +62212,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="177" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>2</v>
       </c>
@@ -62192,7 +62220,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="178" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>3</v>
       </c>
@@ -62200,7 +62228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>4</v>
       </c>
@@ -62208,7 +62236,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="180" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>5</v>
       </c>
@@ -62216,7 +62244,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="181" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>7</v>
       </c>
@@ -62224,7 +62252,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="182" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>9</v>
       </c>
@@ -62232,7 +62260,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="183" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>11</v>
       </c>
@@ -62240,12 +62268,12 @@
         <v>349</v>
       </c>
     </row>
-    <row r="184" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="185" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>13</v>
       </c>
@@ -62277,7 +62305,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="186" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>347</v>
       </c>
@@ -62300,7 +62328,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="187" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
         <v>323</v>
       </c>
@@ -62323,7 +62351,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="188" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>28</v>
       </c>
@@ -62343,7 +62371,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="189" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>328</v>
       </c>
@@ -62363,7 +62391,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="190" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>330</v>
       </c>
@@ -62383,7 +62411,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="191" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>332</v>
       </c>
@@ -62403,7 +62431,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="192" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>334</v>
       </c>
@@ -62423,7 +62451,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="193" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>336</v>
       </c>
@@ -62443,7 +62471,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="194" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>338</v>
       </c>
@@ -62463,7 +62491,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="195" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>100</v>
       </c>
@@ -62483,7 +62511,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="196" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>340</v>
       </c>
@@ -62503,7 +62531,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="197" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>342</v>
       </c>
@@ -62523,8 +62551,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="198" spans="1:10" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="199" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>1</v>
       </c>
@@ -62532,7 +62559,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="200" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>2</v>
       </c>
@@ -62540,7 +62567,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="201" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>3</v>
       </c>
@@ -62548,7 +62575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>4</v>
       </c>
@@ -62556,7 +62583,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="203" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>5</v>
       </c>
@@ -62564,7 +62591,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="204" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>7</v>
       </c>
@@ -62572,7 +62599,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="205" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>9</v>
       </c>
@@ -62580,7 +62607,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="206" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>11</v>
       </c>
@@ -62588,12 +62615,12 @@
         <v>495</v>
       </c>
     </row>
-    <row r="207" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="208" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>13</v>
       </c>
@@ -62625,7 +62652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="209" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>527</v>
       </c>
@@ -62648,7 +62675,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="210" spans="1:10" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A210" s="2" t="s">
         <v>524</v>
       </c>
@@ -62671,7 +62698,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="211" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>28</v>
       </c>
@@ -62691,7 +62718,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="212" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>328</v>
       </c>
@@ -62711,7 +62738,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="213" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>330</v>
       </c>
@@ -62731,7 +62758,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="214" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>332</v>
       </c>
@@ -62751,7 +62778,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="215" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>334</v>
       </c>
@@ -62771,7 +62798,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="216" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>336</v>
       </c>
@@ -62791,7 +62818,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="217" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>338</v>
       </c>
@@ -62811,7 +62838,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="218" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>100</v>
       </c>
@@ -62831,7 +62858,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="219" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>340</v>
       </c>
@@ -62851,7 +62878,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="220" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>342</v>
       </c>
@@ -62872,13 +62899,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J220" xr:uid="{00000000-0001-0000-0200-000000000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Water, unspecified natural origin"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J220" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="G80" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
     <hyperlink ref="G79" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
@@ -65343,7 +65364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N1111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A542" workbookViewId="0">
+    <sheetView topLeftCell="A542" workbookViewId="0">
       <selection activeCell="A571" sqref="A571"/>
     </sheetView>
   </sheetViews>
@@ -85540,10 +85561,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F5820A-E001-4A42-8382-32FC181BB2BB}">
-  <dimension ref="A1:H200"/>
+  <dimension ref="A1:H235"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
+      <selection activeCell="B202" sqref="B202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -87702,8 +87723,8 @@
         <v>69</v>
       </c>
       <c r="B153" s="3">
-        <f>1000*$B$149*(Parameters!B7/5728)</f>
-        <v>1.9401623692733996</v>
+        <f>1000*$B$149*(Parameters!B7/2524)</f>
+        <v>4.4030309236125333</v>
       </c>
       <c r="C153" t="s">
         <v>558</v>
@@ -87723,8 +87744,8 @@
         <v>252</v>
       </c>
       <c r="B154" s="3">
-        <f>1.8*$B$149*(Parameters!B7/5728)</f>
-        <v>3.4922922646921191E-3</v>
+        <f>1.8*$B$149*(Parameters!B7/2524)</f>
+        <v>7.9254556625025594E-3</v>
       </c>
       <c r="C154" t="s">
         <v>558</v>
@@ -87744,8 +87765,8 @@
         <v>376</v>
       </c>
       <c r="B155" s="3">
-        <f>0.45*$B$149*(Parameters!B7/5728)</f>
-        <v>8.7307306617302976E-4</v>
+        <f>0.45*$B$149*(Parameters!B7/2524)</f>
+        <v>1.9813639156256399E-3</v>
       </c>
       <c r="C155" t="s">
         <v>26</v>
@@ -87765,8 +87786,8 @@
         <v>338</v>
       </c>
       <c r="B156" s="3">
-        <f>77.2*$B$149*(Parameters!B7/5728)</f>
-        <v>0.14978053490790647</v>
+        <f>77.2*$B$149*(Parameters!B7/2524)</f>
+        <v>0.33991398730288758</v>
       </c>
       <c r="C156" t="s">
         <v>610</v>
@@ -87786,8 +87807,8 @@
         <v>669</v>
       </c>
       <c r="B157" s="3">
-        <f>5.5*$B$149*(Parameters!B7/5728)</f>
-        <v>1.0670893031003697E-2</v>
+        <f>5.5*$B$149*(Parameters!B7/2524)</f>
+        <v>2.4216670079868934E-2</v>
       </c>
       <c r="C157" t="s">
         <v>31</v>
@@ -87807,8 +87828,8 @@
         <v>1095</v>
       </c>
       <c r="B158" s="3">
-        <f>1.1*$B$149*(Parameters!B7/5728)</f>
-        <v>2.1341786062007398E-3</v>
+        <f>1.1*$B$149*(Parameters!B7/2524)</f>
+        <v>4.8433340159737869E-3</v>
       </c>
       <c r="C158" t="s">
         <v>26</v>
@@ -87828,8 +87849,8 @@
         <v>1097</v>
       </c>
       <c r="B159" s="3">
-        <f>6.8*$B$149*(Parameters!B7/5728)</f>
-        <v>1.3193104111059116E-2</v>
+        <f>6.8*$B$149*(Parameters!B7/2524)</f>
+        <v>2.9940610280565223E-2</v>
       </c>
       <c r="C159" t="s">
         <v>26</v>
@@ -87849,8 +87870,8 @@
         <v>1099</v>
       </c>
       <c r="B160" s="3">
-        <f>0.00000102*$B$149*(Parameters!B7/5728)</f>
-        <v>1.9789656166588675E-9</v>
+        <f>0.00000102*$B$149*(Parameters!B7/2524)</f>
+        <v>4.4910915420847837E-9</v>
       </c>
       <c r="C160" t="s">
         <v>26</v>
@@ -87870,8 +87891,8 @@
         <v>1101</v>
       </c>
       <c r="B161" s="3">
-        <f>0.000000503*$B$149*(Parameters!B7/5728)</f>
-        <v>9.7590167174451989E-10</v>
+        <f>0.000000503*$B$149*(Parameters!B7/2524)</f>
+        <v>2.214724554577104E-9</v>
       </c>
       <c r="C161" t="s">
         <v>26</v>
@@ -87891,8 +87912,8 @@
         <v>265</v>
       </c>
       <c r="B162" s="3">
-        <f>('Cavalett &amp; Cherubini 2022'!B153*'Cozzolini 2018'!$B$569)-Parameters!$B$17</f>
-        <v>0.37850862891855597</v>
+        <f>(B153*1.81)-3.15</f>
+        <v>4.8194859717386862</v>
       </c>
       <c r="D162" t="s">
         <v>8</v>
@@ -87902,6 +87923,9 @@
       </c>
       <c r="F162" t="s">
         <v>36</v>
+      </c>
+      <c r="G162" t="s">
+        <v>1151</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
@@ -87909,8 +87933,8 @@
         <v>191</v>
       </c>
       <c r="B163" s="6">
-        <f>0.000441*$B$149*(Parameters!B7/5728)</f>
-        <v>8.5561160484956925E-7</v>
+        <f>0.000441*$B$149*(Parameters!B7/2524)</f>
+        <v>1.9417366373131271E-6</v>
       </c>
       <c r="D163" t="s">
         <v>8</v>
@@ -87927,8 +87951,8 @@
         <v>193</v>
       </c>
       <c r="B164" s="6">
-        <f>0.00042*$B$149*(Parameters!B7/5728)</f>
-        <v>8.1486819509482783E-7</v>
+        <f>0.00042*$B$149*(Parameters!B7/2524)</f>
+        <v>1.849272987917264E-6</v>
       </c>
       <c r="D164" t="s">
         <v>8</v>
@@ -87945,8 +87969,8 @@
         <v>38</v>
       </c>
       <c r="B165" s="6">
-        <f>0.00376*$B$149*(Parameters!B7/5728)</f>
-        <v>7.2950105084679824E-6</v>
+        <f>0.00376*$B$149*(Parameters!B7/2524)</f>
+        <v>1.6555396272783125E-5</v>
       </c>
       <c r="D165" t="s">
         <v>8</v>
@@ -87963,8 +87987,8 @@
         <v>314</v>
       </c>
       <c r="B166" s="6">
-        <f>0.000115*$B$149*(Parameters!B7/5728)</f>
-        <v>2.2311867246644096E-7</v>
+        <f>0.000115*$B$149*(Parameters!B7/2524)</f>
+        <v>5.0634855621544133E-7</v>
       </c>
       <c r="D166" t="s">
         <v>8</v>
@@ -87981,8 +88005,8 @@
         <v>315</v>
       </c>
       <c r="B167" s="6">
-        <f>0.000042*$B$149*(Parameters!B7/5728)</f>
-        <v>8.1486819509482786E-8</v>
+        <f>0.000042*$B$149*(Parameters!B7/2524)</f>
+        <v>1.849272987917264E-7</v>
       </c>
       <c r="D167" t="s">
         <v>8</v>
@@ -87999,8 +88023,8 @@
         <v>40</v>
       </c>
       <c r="B168" s="6">
-        <f>0.000021*$B$149*(Parameters!B7/5728)</f>
-        <v>4.0743409754741393E-8</v>
+        <f>0.000021*$B$149*(Parameters!B7/2524)</f>
+        <v>9.2463649395863201E-8</v>
       </c>
       <c r="D168" t="s">
         <v>8</v>
@@ -88017,7 +88041,7 @@
         <v>1</v>
       </c>
       <c r="B170" s="58" t="s">
-        <v>1108</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
@@ -88135,7 +88159,7 @@
     </row>
     <row r="184" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>1108</v>
+        <v>1150</v>
       </c>
       <c r="B184" s="3">
         <v>1</v>
@@ -88161,8 +88185,8 @@
         <v>1090</v>
       </c>
       <c r="B185" s="3">
-        <f>1000*$B$181*(Parameters!B7/5728)</f>
-        <v>1.9401623692733996</v>
+        <f>1000*$B$181*(Parameters!B7/2524)</f>
+        <v>4.4030309236125333</v>
       </c>
       <c r="C185" t="s">
         <v>558</v>
@@ -88182,8 +88206,8 @@
         <v>252</v>
       </c>
       <c r="B186" s="3">
-        <f>1.8*$B$181*(Parameters!B7/5728)</f>
-        <v>3.4922922646921191E-3</v>
+        <f>1.8*$B$181*(Parameters!B7/2524)</f>
+        <v>7.9254556625025594E-3</v>
       </c>
       <c r="C186" t="s">
         <v>558</v>
@@ -88203,8 +88227,8 @@
         <v>376</v>
       </c>
       <c r="B187" s="3">
-        <f>0.45*$B$181*(Parameters!B7/5728)</f>
-        <v>8.7307306617302976E-4</v>
+        <f>0.45*$B$181*(Parameters!B7/2524)</f>
+        <v>1.9813639156256399E-3</v>
       </c>
       <c r="C187" t="s">
         <v>26</v>
@@ -88224,8 +88248,8 @@
         <v>338</v>
       </c>
       <c r="B188" s="3">
-        <f>77.2*$B$181*(Parameters!B7/5728)</f>
-        <v>0.14978053490790647</v>
+        <f>77.2*$B$181*(Parameters!B7/2524)</f>
+        <v>0.33991398730288758</v>
       </c>
       <c r="C188" t="s">
         <v>610</v>
@@ -88245,8 +88269,8 @@
         <v>669</v>
       </c>
       <c r="B189" s="3">
-        <f>5.5*$B$181*(Parameters!B7/5728)</f>
-        <v>1.0670893031003697E-2</v>
+        <f>5.5*$B$181*(Parameters!B7/2524)</f>
+        <v>2.4216670079868934E-2</v>
       </c>
       <c r="C189" t="s">
         <v>31</v>
@@ -88266,8 +88290,8 @@
         <v>1095</v>
       </c>
       <c r="B190" s="3">
-        <f>1.1*$B$181*(Parameters!B7/5728)</f>
-        <v>2.1341786062007398E-3</v>
+        <f>1.1*$B$181*(Parameters!B7/2524)</f>
+        <v>4.8433340159737869E-3</v>
       </c>
       <c r="C190" t="s">
         <v>26</v>
@@ -88287,8 +88311,8 @@
         <v>1097</v>
       </c>
       <c r="B191" s="3">
-        <f>6.8*$B$181*(Parameters!B7/5728)</f>
-        <v>1.3193104111059116E-2</v>
+        <f>6.8*$B$181*(Parameters!B7/2524)</f>
+        <v>2.9940610280565223E-2</v>
       </c>
       <c r="C191" t="s">
         <v>26</v>
@@ -88308,8 +88332,8 @@
         <v>1099</v>
       </c>
       <c r="B192" s="3">
-        <f>0.00000102*$B$181*(Parameters!B7/5728)</f>
-        <v>1.9789656166588675E-9</v>
+        <f>0.00000102*$B$181*(Parameters!B7/2524)</f>
+        <v>4.4910915420847837E-9</v>
       </c>
       <c r="C192" t="s">
         <v>26</v>
@@ -88329,8 +88353,8 @@
         <v>1101</v>
       </c>
       <c r="B193" s="3">
-        <f>0.000000503*$B$181*(Parameters!B7/5728)</f>
-        <v>9.7590167174451989E-10</v>
+        <f>0.000000503*$B$181*(Parameters!B7/2524)</f>
+        <v>2.214724554577104E-9</v>
       </c>
       <c r="C193" t="s">
         <v>26</v>
@@ -88350,8 +88374,8 @@
         <v>265</v>
       </c>
       <c r="B194" s="3">
-        <f>('Cavalett &amp; Cherubini 2022'!B185*'Cozzolini 2018'!$B$569)-Parameters!$B$17</f>
-        <v>0.37850862891855597</v>
+        <f>(B185*1.81)-3.15</f>
+        <v>4.8194859717386862</v>
       </c>
       <c r="D194" t="s">
         <v>8</v>
@@ -88368,8 +88392,8 @@
         <v>191</v>
       </c>
       <c r="B195" s="6">
-        <f>0.000441*$B$181*(Parameters!B7/5728)</f>
-        <v>8.5561160484956925E-7</v>
+        <f>0.000441*$B$181*(Parameters!B7/2524)</f>
+        <v>1.9417366373131271E-6</v>
       </c>
       <c r="D195" t="s">
         <v>8</v>
@@ -88386,8 +88410,8 @@
         <v>193</v>
       </c>
       <c r="B196" s="6">
-        <f>0.00042*$B$181*(Parameters!B7/5728)</f>
-        <v>8.1486819509482783E-7</v>
+        <f>0.00042*$B$181*(Parameters!B7/2524)</f>
+        <v>1.849272987917264E-6</v>
       </c>
       <c r="D196" t="s">
         <v>8</v>
@@ -88404,8 +88428,8 @@
         <v>38</v>
       </c>
       <c r="B197" s="6">
-        <f>0.00376*$B$181*(Parameters!B7/5728)</f>
-        <v>7.2950105084679824E-6</v>
+        <f>0.00376*$B$181*(Parameters!B7/2524)</f>
+        <v>1.6555396272783125E-5</v>
       </c>
       <c r="D197" t="s">
         <v>8</v>
@@ -88422,8 +88446,8 @@
         <v>314</v>
       </c>
       <c r="B198" s="6">
-        <f>0.000115*$B$181*(Parameters!B7/5728)</f>
-        <v>2.2311867246644096E-7</v>
+        <f>0.000115*$B$181*(Parameters!B7/2524)</f>
+        <v>5.0634855621544133E-7</v>
       </c>
       <c r="D198" t="s">
         <v>8</v>
@@ -88440,8 +88464,8 @@
         <v>315</v>
       </c>
       <c r="B199" s="6">
-        <f>0.000042*$B$181*(Parameters!B7/5728)</f>
-        <v>8.1486819509482786E-8</v>
+        <f>0.000042*$B$181*(Parameters!B7/2524)</f>
+        <v>1.849272987917264E-7</v>
       </c>
       <c r="D199" t="s">
         <v>8</v>
@@ -88458,8 +88482,8 @@
         <v>40</v>
       </c>
       <c r="B200" s="6">
-        <f>0.000021*$B$181*(Parameters!B7/5728)</f>
-        <v>4.0743409754741393E-8</v>
+        <f>0.000021*$B$181*(Parameters!B7/2524)</f>
+        <v>9.2463649395863201E-8</v>
       </c>
       <c r="D200" t="s">
         <v>8</v>
@@ -88469,11 +88493,527 @@
       </c>
       <c r="F200" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A202" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B202" s="58" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>2</v>
+      </c>
+      <c r="B203" s="6" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>3</v>
+      </c>
+      <c r="B204" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>4</v>
+      </c>
+      <c r="B205" s="67" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>5</v>
+      </c>
+      <c r="B206" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>7</v>
+      </c>
+      <c r="B207" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>9</v>
+      </c>
+      <c r="B208" s="6" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>11</v>
+      </c>
+      <c r="B209" s="5"/>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B210" s="5"/>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B211" s="5"/>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>485</v>
+      </c>
+      <c r="B212" s="66"/>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B213" s="28">
+        <f>2524/(5728+1514+2524)</f>
+        <v>0.25844767560925658</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A214" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B214" s="6"/>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>13</v>
+      </c>
+      <c r="B215" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C215" t="s">
+        <v>2</v>
+      </c>
+      <c r="D215" t="s">
+        <v>7</v>
+      </c>
+      <c r="E215" t="s">
+        <v>15</v>
+      </c>
+      <c r="F215" t="s">
+        <v>5</v>
+      </c>
+      <c r="G215" t="s">
+        <v>11</v>
+      </c>
+      <c r="H215" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A216" s="6" t="str">
+        <f>B202</f>
+        <v>kerosene production, via Fischer-Tropsch, from forest product (non-residual), with carbon capture and storage, energy allocation</v>
+      </c>
+      <c r="B216" s="3">
+        <v>1</v>
+      </c>
+      <c r="C216" t="s">
+        <v>558</v>
+      </c>
+      <c r="D216" t="s">
+        <v>8</v>
+      </c>
+      <c r="F216" t="s">
+        <v>17</v>
+      </c>
+      <c r="G216" t="s">
+        <v>18</v>
+      </c>
+      <c r="H216" s="67" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B217" s="3">
+        <v>4.4030309236125333</v>
+      </c>
+      <c r="C217" t="s">
+        <v>558</v>
+      </c>
+      <c r="D217" t="s">
+        <v>8</v>
+      </c>
+      <c r="F217" t="s">
+        <v>20</v>
+      </c>
+      <c r="H217" s="6" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>252</v>
+      </c>
+      <c r="B218" s="3">
+        <v>7.9254556625025594E-3</v>
+      </c>
+      <c r="C218" t="s">
+        <v>558</v>
+      </c>
+      <c r="D218" t="s">
+        <v>8</v>
+      </c>
+      <c r="F218" t="s">
+        <v>20</v>
+      </c>
+      <c r="H218" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>376</v>
+      </c>
+      <c r="B219" s="3">
+        <v>1.9813639156256399E-3</v>
+      </c>
+      <c r="C219" t="s">
+        <v>26</v>
+      </c>
+      <c r="D219" t="s">
+        <v>8</v>
+      </c>
+      <c r="F219" t="s">
+        <v>20</v>
+      </c>
+      <c r="H219" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>338</v>
+      </c>
+      <c r="B220" s="3">
+        <v>0.33991398730288758</v>
+      </c>
+      <c r="C220" t="s">
+        <v>610</v>
+      </c>
+      <c r="D220" t="s">
+        <v>8</v>
+      </c>
+      <c r="F220" t="s">
+        <v>20</v>
+      </c>
+      <c r="H220" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>669</v>
+      </c>
+      <c r="B221" s="3">
+        <v>2.4216670079868934E-2</v>
+      </c>
+      <c r="C221" t="s">
+        <v>31</v>
+      </c>
+      <c r="D221" t="s">
+        <v>8</v>
+      </c>
+      <c r="F221" t="s">
+        <v>20</v>
+      </c>
+      <c r="H221" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B222" s="3">
+        <v>4.8433340159737869E-3</v>
+      </c>
+      <c r="C222" t="s">
+        <v>26</v>
+      </c>
+      <c r="D222" t="s">
+        <v>8</v>
+      </c>
+      <c r="F222" t="s">
+        <v>20</v>
+      </c>
+      <c r="H222" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B223" s="3">
+        <v>2.9940610280565223E-2</v>
+      </c>
+      <c r="C223" t="s">
+        <v>26</v>
+      </c>
+      <c r="D223" t="s">
+        <v>8</v>
+      </c>
+      <c r="F223" t="s">
+        <v>20</v>
+      </c>
+      <c r="H223" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B224" s="3">
+        <v>4.4910915420847837E-9</v>
+      </c>
+      <c r="C224" t="s">
+        <v>26</v>
+      </c>
+      <c r="D224" t="s">
+        <v>7</v>
+      </c>
+      <c r="F224" t="s">
+        <v>20</v>
+      </c>
+      <c r="H224" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B225" s="3">
+        <v>2.214724554577104E-9</v>
+      </c>
+      <c r="C225" t="s">
+        <v>26</v>
+      </c>
+      <c r="D225" t="s">
+        <v>7</v>
+      </c>
+      <c r="F225" t="s">
+        <v>20</v>
+      </c>
+      <c r="H225" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>265</v>
+      </c>
+      <c r="B226" s="3">
+        <f>4.81948597173869*0.1</f>
+        <v>0.48194859717386901</v>
+      </c>
+      <c r="D226" t="s">
+        <v>8</v>
+      </c>
+      <c r="E226" t="s">
+        <v>37</v>
+      </c>
+      <c r="F226" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>191</v>
+      </c>
+      <c r="B227" s="6">
+        <v>1.9417366373131271E-6</v>
+      </c>
+      <c r="D227" t="s">
+        <v>8</v>
+      </c>
+      <c r="E227" t="s">
+        <v>37</v>
+      </c>
+      <c r="F227" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>193</v>
+      </c>
+      <c r="B228" s="6">
+        <v>1.849272987917264E-6</v>
+      </c>
+      <c r="D228" t="s">
+        <v>8</v>
+      </c>
+      <c r="E228" t="s">
+        <v>37</v>
+      </c>
+      <c r="F228" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>38</v>
+      </c>
+      <c r="B229" s="6">
+        <v>1.6555396272783125E-5</v>
+      </c>
+      <c r="D229" t="s">
+        <v>8</v>
+      </c>
+      <c r="E229" t="s">
+        <v>37</v>
+      </c>
+      <c r="F229" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>314</v>
+      </c>
+      <c r="B230" s="6">
+        <v>5.0634855621544133E-7</v>
+      </c>
+      <c r="D230" t="s">
+        <v>8</v>
+      </c>
+      <c r="E230" t="s">
+        <v>37</v>
+      </c>
+      <c r="F230" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>315</v>
+      </c>
+      <c r="B231" s="6">
+        <v>1.849272987917264E-7</v>
+      </c>
+      <c r="D231" t="s">
+        <v>8</v>
+      </c>
+      <c r="E231" t="s">
+        <v>37</v>
+      </c>
+      <c r="F231" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>40</v>
+      </c>
+      <c r="B232" s="6">
+        <v>9.2463649395863201E-8</v>
+      </c>
+      <c r="D232" t="s">
+        <v>8</v>
+      </c>
+      <c r="E232" t="s">
+        <v>37</v>
+      </c>
+      <c r="F232" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>28</v>
+      </c>
+      <c r="B233" s="6">
+        <v>0.23</v>
+      </c>
+      <c r="C233" t="s">
+        <v>558</v>
+      </c>
+      <c r="D233" t="s">
+        <v>29</v>
+      </c>
+      <c r="F233" t="s">
+        <v>20</v>
+      </c>
+      <c r="G233" t="s">
+        <v>1153</v>
+      </c>
+      <c r="H233" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B234" s="6">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C234" t="s">
+        <v>26</v>
+      </c>
+      <c r="D234" t="s">
+        <v>8</v>
+      </c>
+      <c r="F234" t="s">
+        <v>20</v>
+      </c>
+      <c r="G234" t="s">
+        <v>1156</v>
+      </c>
+      <c r="H234" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B235" s="71">
+        <f>4.81948597173869*0.9</f>
+        <v>4.3375373745648211</v>
+      </c>
+      <c r="C235" t="s">
+        <v>558</v>
+      </c>
+      <c r="D235" t="s">
+        <v>8</v>
+      </c>
+      <c r="F235" t="s">
+        <v>20</v>
+      </c>
+      <c r="G235" t="s">
+        <v>1159</v>
+      </c>
+      <c r="H235" t="s">
+        <v>1158</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H200" xr:uid="{06F5820A-E001-4A42-8382-32FC181BB2BB}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fix issue with efficiency scaling for lignite power plants
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-biofuels.xlsx
+++ b/premise/data/additional_inventories/lci-biofuels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D0E443-966E-754B-B87A-558D22ECBC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DE8EE5-0845-EB4F-98B0-880A61010560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -580,7 +580,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19437" uniqueCount="1161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19437" uniqueCount="1162">
   <si>
     <t>Database</t>
   </si>
@@ -4091,6 +4091,9 @@
   </si>
   <si>
     <t>irrigation, from "sweet sorghum production, CN" from ecoinvent</t>
+  </si>
+  <si>
+    <t>from ecoinvent 3.7 "rape seed production, DE"</t>
   </si>
 </sst>
 </file>
@@ -4765,8 +4768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W166"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="B16" zoomScale="82" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+    <sheetView showZeros="0" topLeftCell="B1" zoomScale="82" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13531,7 +13534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J2872"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2008" zoomScale="131" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView topLeftCell="B2008" zoomScale="131" zoomScaleNormal="78" workbookViewId="0">
       <selection activeCell="G2024" sqref="G2024"/>
     </sheetView>
   </sheetViews>
@@ -65353,8 +65356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N1111"/>
   <sheetViews>
-    <sheetView topLeftCell="A542" workbookViewId="0">
-      <selection activeCell="A571" sqref="A571"/>
+    <sheetView tabSelected="1" topLeftCell="A717" workbookViewId="0">
+      <selection activeCell="G755" sqref="G755"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -78957,7 +78960,7 @@
         <v>126</v>
       </c>
       <c r="B754" s="6">
-        <v>0.21836674491491001</v>
+        <v>7.6053367504319305E-2</v>
       </c>
       <c r="D754" t="s">
         <v>121</v>
@@ -78969,7 +78972,7 @@
         <v>36</v>
       </c>
       <c r="G754" t="s">
-        <v>940</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="755" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update final energy mapping.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-biofuels.xlsx
+++ b/premise/data/additional_inventories/lci-biofuels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942994E7-6F34-8448-AF47-7B1EAC61FEB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5506ECCF-EE0D-6146-9E99-FA47F147A979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2320" windowWidth="36080" windowHeight="22720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -580,7 +580,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19441" uniqueCount="1161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19446" uniqueCount="1163">
   <si>
     <t>Database</t>
   </si>
@@ -4051,9 +4051,6 @@
     <t>kerosene production, via Fischer-Tropsch, from forest product (non-residual), energy allocation</t>
   </si>
   <si>
-    <t>1.81kg CO2/kg wood chips. Kerosene: 3.15 kgCO2/kg</t>
-  </si>
-  <si>
     <t>kerosene production, via Fischer-Tropsch, from forest product (non-residual), with carbon capture and storage, energy allocation</t>
   </si>
   <si>
@@ -4091,6 +4088,15 @@
   </si>
   <si>
     <t>0 km by barge, 150 km by truck.</t>
+  </si>
+  <si>
+    <t>1.86kg CO2/kg wood chips. Kerosene: 3.1 kgCO2/kg</t>
+  </si>
+  <si>
+    <t>1.86kg CO2/kg wood chips. Biodiesel: 2.8 kgCO2/kg</t>
+  </si>
+  <si>
+    <t>1.86kg CO2/kg wood chips. Ethanol: 1.91 kgCO2/kg</t>
   </si>
 </sst>
 </file>
@@ -4485,7 +4491,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -7298,7 +7304,7 @@
       </c>
       <c r="M53" s="5">
         <f>'Cavalett &amp; Cherubini 2022'!B27</f>
-        <v>5.1810216734533041</v>
+        <v>5.3462721660317882</v>
       </c>
       <c r="N53">
         <v>26.8</v>
@@ -7344,7 +7350,7 @@
       </c>
       <c r="M54" s="5">
         <f>'Cavalett &amp; Cherubini 2022'!B63</f>
-        <v>5.1810216734533041</v>
+        <v>5.3462721660317882</v>
       </c>
       <c r="N54">
         <v>26.8</v>
@@ -7595,7 +7601,7 @@
       </c>
       <c r="M59" s="5">
         <f>'Cavalett &amp; Cherubini 2022'!B97</f>
-        <v>4.0775445422895764</v>
+        <v>4.2849887364325214</v>
       </c>
       <c r="N59">
         <v>43</v>
@@ -7641,7 +7647,7 @@
       </c>
       <c r="M60" s="5">
         <f>'Cavalett &amp; Cherubini 2022'!B129</f>
-        <v>4.0775445422895764</v>
+        <v>4.2849887364325214</v>
       </c>
       <c r="N60">
         <v>43</v>
@@ -7687,7 +7693,7 @@
       </c>
       <c r="M61" s="5">
         <f>'Cavalett &amp; Cherubini 2022'!B162</f>
-        <v>4.8194859717386862</v>
+        <v>5.0896375179193125</v>
       </c>
       <c r="N61">
         <v>43</v>
@@ -7733,7 +7739,7 @@
       </c>
       <c r="M62" s="5">
         <f>'Cavalett &amp; Cherubini 2022'!B194</f>
-        <v>4.8194859717386862</v>
+        <v>5.0896375179193125</v>
       </c>
       <c r="N62">
         <v>43</v>
@@ -8986,7 +8992,7 @@
       </c>
       <c r="M86" s="4">
         <f t="shared" si="20"/>
-        <v>0.19332170423333223</v>
+        <v>0.19948776738924581</v>
       </c>
       <c r="N86" s="35">
         <f t="shared" si="21"/>
@@ -9044,7 +9050,7 @@
       </c>
       <c r="M87" s="4">
         <f t="shared" si="20"/>
-        <v>0.19332170423333223</v>
+        <v>0.19948776738924581</v>
       </c>
       <c r="N87" s="35">
         <f t="shared" si="21"/>
@@ -9334,7 +9340,7 @@
       </c>
       <c r="M92" s="4">
         <f t="shared" si="20"/>
-        <v>9.4826617262548291E-2</v>
+        <v>9.9650900847267937E-2</v>
       </c>
       <c r="N92" s="35">
         <f t="shared" si="21"/>
@@ -9392,7 +9398,7 @@
       </c>
       <c r="M93" s="4">
         <f t="shared" si="20"/>
-        <v>9.4826617262548291E-2</v>
+        <v>9.9650900847267937E-2</v>
       </c>
       <c r="N93" s="35">
         <f t="shared" si="21"/>
@@ -9450,7 +9456,7 @@
       </c>
       <c r="M94" s="4">
         <f t="shared" si="20"/>
-        <v>0.11208106911020201</v>
+        <v>0.11836366320742588</v>
       </c>
       <c r="N94" s="35">
         <f t="shared" si="21"/>
@@ -9508,7 +9514,7 @@
       </c>
       <c r="M95" s="4">
         <f t="shared" si="20"/>
-        <v>0.11208106911020201</v>
+        <v>0.11836366320742588</v>
       </c>
       <c r="N95" s="35">
         <f t="shared" si="21"/>
@@ -45617,7 +45623,7 @@
         <v>20</v>
       </c>
       <c r="G2023" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="H2023" t="s">
         <v>122</v>
@@ -63332,7 +63338,7 @@
         <v>36</v>
       </c>
       <c r="G27" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
@@ -63353,7 +63359,7 @@
         <v>36</v>
       </c>
       <c r="G28" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
@@ -63374,7 +63380,7 @@
         <v>36</v>
       </c>
       <c r="G29" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -65368,7 +65374,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N1111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A541" workbookViewId="0">
+    <sheetView topLeftCell="A541" workbookViewId="0">
       <selection activeCell="G552" sqref="G552"/>
     </sheetView>
   </sheetViews>
@@ -75594,7 +75600,7 @@
         <v>11</v>
       </c>
       <c r="B561" s="6" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="562" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -78984,7 +78990,7 @@
         <v>36</v>
       </c>
       <c r="G754" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="755" spans="1:8" x14ac:dyDescent="0.2">
@@ -85567,8 +85573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F5820A-E001-4A42-8382-32FC181BB2BB}">
   <dimension ref="A1:H235"/>
   <sheetViews>
-    <sheetView topLeftCell="A212" workbookViewId="0">
-      <selection activeCell="A227" sqref="A227"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -85960,8 +85966,8 @@
         <v>265</v>
       </c>
       <c r="B27" s="3">
-        <f>('Cavalett &amp; Cherubini 2022'!B16*'Cozzolini 2018'!$B$569)-Parameters!$B$15</f>
-        <v>5.1810216734533041</v>
+        <f>(B16*1.86)-1.91</f>
+        <v>5.3462721660317882</v>
       </c>
       <c r="D27" t="s">
         <v>8</v>
@@ -85971,6 +85977,9 @@
       </c>
       <c r="F27" t="s">
         <v>36</v>
+      </c>
+      <c r="G27" t="s">
+        <v>1162</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -86501,8 +86510,8 @@
         <v>265</v>
       </c>
       <c r="B63" s="3">
-        <f>('Cavalett &amp; Cherubini 2022'!B52*'Cozzolini 2018'!$B$569)-Parameters!$B$15</f>
-        <v>5.1810216734533041</v>
+        <f>(B52*1.86)-1.91</f>
+        <v>5.3462721660317882</v>
       </c>
       <c r="D63" t="s">
         <v>8</v>
@@ -86512,6 +86521,9 @@
       </c>
       <c r="F63" t="s">
         <v>36</v>
+      </c>
+      <c r="G63" t="s">
+        <v>1162</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -86993,13 +87005,13 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>265</v>
       </c>
       <c r="B97" s="3">
-        <f>('Cavalett &amp; Cherubini 2022'!B88*'Cozzolini 2018'!$B$569)-Parameters!$B$16</f>
-        <v>4.0775445422895764</v>
+        <f>(B88*1.86)-2.8</f>
+        <v>4.2849887364325214</v>
       </c>
       <c r="D97" t="s">
         <v>8</v>
@@ -87010,8 +87022,11 @@
       <c r="F97" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G97" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>191</v>
       </c>
@@ -87029,7 +87044,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>193</v>
       </c>
@@ -87047,7 +87062,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>38</v>
       </c>
@@ -87065,7 +87080,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>314</v>
       </c>
@@ -87083,7 +87098,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>315</v>
       </c>
@@ -87101,7 +87116,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>40</v>
       </c>
@@ -87119,7 +87134,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>1</v>
       </c>
@@ -87127,7 +87142,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>2</v>
       </c>
@@ -87135,7 +87150,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>3</v>
       </c>
@@ -87143,7 +87158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>4</v>
       </c>
@@ -87151,7 +87166,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>5</v>
       </c>
@@ -87159,7 +87174,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>7</v>
       </c>
@@ -87167,7 +87182,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>9</v>
       </c>
@@ -87175,7 +87190,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>11</v>
       </c>
@@ -87454,13 +87469,13 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>265</v>
       </c>
       <c r="B129" s="3">
-        <f>('Cavalett &amp; Cherubini 2022'!B120*'Cozzolini 2018'!$B$569)-Parameters!$B$16</f>
-        <v>4.0775445422895764</v>
+        <f>(B120*1.86)-2.8</f>
+        <v>4.2849887364325214</v>
       </c>
       <c r="D129" t="s">
         <v>8</v>
@@ -87471,8 +87486,11 @@
       <c r="F129" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G129" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>191</v>
       </c>
@@ -87490,7 +87508,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>193</v>
       </c>
@@ -87508,7 +87526,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>38</v>
       </c>
@@ -87526,7 +87544,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>314</v>
       </c>
@@ -87544,7 +87562,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>315</v>
       </c>
@@ -87562,7 +87580,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>40</v>
       </c>
@@ -87580,7 +87598,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>1</v>
       </c>
@@ -87588,7 +87606,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>2</v>
       </c>
@@ -87596,7 +87614,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>3</v>
       </c>
@@ -87604,7 +87622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>4</v>
       </c>
@@ -87612,7 +87630,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>5</v>
       </c>
@@ -87620,7 +87638,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>7</v>
       </c>
@@ -87628,7 +87646,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>9</v>
       </c>
@@ -87920,8 +87938,8 @@
         <v>265</v>
       </c>
       <c r="B162" s="3">
-        <f>(B153*1.81)-3.15</f>
-        <v>4.8194859717386862</v>
+        <f>(B153*1.86)-3.1</f>
+        <v>5.0896375179193125</v>
       </c>
       <c r="D162" t="s">
         <v>8</v>
@@ -87933,7 +87951,7 @@
         <v>36</v>
       </c>
       <c r="G162" t="s">
-        <v>1147</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
@@ -88384,8 +88402,8 @@
         <v>265</v>
       </c>
       <c r="B194" s="3">
-        <f>(B185*1.81)-3.15</f>
-        <v>4.8194859717386862</v>
+        <f>(B185*1.86)-3.1</f>
+        <v>5.0896375179193125</v>
       </c>
       <c r="D194" t="s">
         <v>8</v>
@@ -88395,6 +88413,9 @@
       </c>
       <c r="F194" t="s">
         <v>36</v>
+      </c>
+      <c r="G194" t="s">
+        <v>1160</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.2">
@@ -88510,7 +88531,7 @@
         <v>1</v>
       </c>
       <c r="B202" s="58" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.2">
@@ -88558,7 +88579,7 @@
         <v>9</v>
       </c>
       <c r="B208" s="6" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.2">
@@ -88969,7 +88990,7 @@
         <v>20</v>
       </c>
       <c r="G233" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="H233" t="s">
         <v>30</v>
@@ -88977,7 +88998,7 @@
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="B234" s="6">
         <v>4.0000000000000001E-3</v>
@@ -88992,15 +89013,15 @@
         <v>20</v>
       </c>
       <c r="G234" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="H234" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B235" s="71">
         <f>4.81948597173869*0.9</f>
@@ -89016,10 +89037,10 @@
         <v>20</v>
       </c>
       <c r="G235" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="H235" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>